<commit_message>
fresh api calls, extra vars from census and cdc
</commit_message>
<xml_diff>
--- a/2_clean/secondary_metrics.xlsx
+++ b/2_clean/secondary_metrics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvmoffice-my.sharepoint.com/personal/swalshda_uvm_edu/Documents/Food Systems Research Center/Sustainability Metrics/Sustainability Metrics Manuscript/Metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3315" documentId="11_DCEFBFC18F79A8D366075C52F37BD2728ACE46B3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C3D9E70-52AC-4905-8665-071BF85AE46A}"/>
+  <xr:revisionPtr revIDLastSave="3334" documentId="11_DCEFBFC18F79A8D366075C52F37BD2728ACE46B3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5E3997F-FD94-43D6-923C-F25126D3989A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1860" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="14592" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Economics" sheetId="3" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="514">
   <si>
     <t>quality</t>
   </si>
@@ -389,9 +389,6 @@
     <t>Air pollution - particulate matter</t>
   </si>
   <si>
-    <t>airPollutionParticulateMatter</t>
-  </si>
-  <si>
     <t>Total CH4 emissions from agriculture (Tg)</t>
   </si>
   <si>
@@ -608,6 +605,9 @@
     <t>https://www.mrlc.gov/data/type/land-cover</t>
   </si>
   <si>
+    <t>Shannon index of LULC types with some grouping - forests, high and low development, wetlands, grasslands and shrubs</t>
+  </si>
+  <si>
     <t>lulcDiversity</t>
   </si>
   <si>
@@ -626,13 +626,16 @@
     <t>water quality</t>
   </si>
   <si>
+    <t>Lake habitat complexity condition class</t>
+  </si>
+  <si>
     <t>U.S. Environmental Protection Agency, National Aquatic Resource Surveys, 2022</t>
   </si>
   <si>
     <t>https://www.epa.gov/national-aquatic-resource-surveys/data-national-aquatic-resource-surveys</t>
   </si>
   <si>
-    <t>Lake habitat complexity condition class</t>
+    <t>could use better source - categorical, and state level only</t>
   </si>
   <si>
     <t>lakesLitripcvrCond</t>
@@ -653,42 +656,51 @@
     <t>water quantity</t>
   </si>
   <si>
+    <t>Precipitation</t>
+  </si>
+  <si>
+    <t>monthly</t>
+  </si>
+  <si>
+    <t>PRISM Group, Oregon State University (2025).</t>
+  </si>
+  <si>
+    <t>https://www.prism.oregonstate.edu/recent/</t>
+  </si>
+  <si>
+    <t>Not sure if this is necessary. Could use SPEI?</t>
+  </si>
+  <si>
+    <t>Weeks of extreme drought</t>
+  </si>
+  <si>
+    <t>weekly</t>
+  </si>
+  <si>
+    <t>U.S. Department of Agriculture, U.S. Drought Monitor. (2024).</t>
+  </si>
+  <si>
+    <t>https://droughtmonitor.unl.edu/DmData/DataDownload.aspx</t>
+  </si>
+  <si>
+    <t>This is tabular pulled from API, but they also have rasters and vectors</t>
+  </si>
+  <si>
+    <t>droughtNonConWeeksCat2</t>
+  </si>
+  <si>
+    <t>soils</t>
+  </si>
+  <si>
+    <t>biology</t>
+  </si>
+  <si>
+    <t>Limitations for aerobic soil organisms</t>
+  </si>
+  <si>
     <t>vector</t>
   </si>
   <si>
-    <t>weekly</t>
-  </si>
-  <si>
-    <t>U.S. Department of Agriculture, U.S. Drought Monitor. (2024).</t>
-  </si>
-  <si>
-    <t>https://droughtmonitor.unl.edu/DmData/DataDownload.aspx</t>
-  </si>
-  <si>
-    <t>Precipitation</t>
-  </si>
-  <si>
-    <t>monthly</t>
-  </si>
-  <si>
-    <t>PRISM Group, Oregon State University (2025).</t>
-  </si>
-  <si>
-    <t>https://www.prism.oregonstate.edu/recent/</t>
-  </si>
-  <si>
-    <t>Weeks of extreme drought</t>
-  </si>
-  <si>
-    <t>soils</t>
-  </si>
-  <si>
-    <t>biology</t>
-  </si>
-  <si>
-    <t>Limitations for aerobic soil organisms</t>
-  </si>
-  <si>
     <t>?</t>
   </si>
   <si>
@@ -1067,6 +1079,9 @@
     <t>product quality tbd</t>
   </si>
   <si>
+    <t>FDA recalls?</t>
+  </si>
+  <si>
     <t>product safety (not livestock)</t>
   </si>
   <si>
@@ -1208,9 +1223,6 @@
     <t>Social associations</t>
   </si>
   <si>
-    <t>See Rupasingha 2006 - BLS lists establishments by NAICS code, weight by population.</t>
-  </si>
-  <si>
     <t>socialAssociations</t>
   </si>
   <si>
@@ -1562,22 +1574,22 @@
     <t>Only for SFA metrics</t>
   </si>
   <si>
-    <t>FDA recalls?</t>
-  </si>
-  <si>
-    <t>This is tabular pulled from API, but they also have rasters and vectors</t>
-  </si>
-  <si>
-    <t>Not sure if this is necessary. Could use SPEI?</t>
-  </si>
-  <si>
-    <t>Shannon index of LULC types with some grouping - forests, high and low development, wetlands, grasslands and shrubs</t>
-  </si>
-  <si>
-    <t>could use better source - categorical, and state level only</t>
-  </si>
-  <si>
-    <t>droughtNonConWeeksCat2</t>
+    <t>Lots of data from CDC EPH Tracking network. Could use some suggestions on which diseases. Diabetes, cholesterol</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>CDC Environmental Public Health Tracking</t>
+  </si>
+  <si>
+    <t>https://ephtracking.cdc.gov/</t>
+  </si>
+  <si>
+    <t>consider weighting by population</t>
+  </si>
+  <si>
+    <t>airQuality</t>
   </si>
 </sst>
 </file>
@@ -2509,7 +2521,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3494,6 +3506,7 @@
     <sortCondition ref="C2:C30"/>
     <sortCondition ref="D2:D30"/>
   </sortState>
+  <dataConsolidate/>
   <mergeCells count="10">
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="B2:B5"/>
@@ -3520,8 +3533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802AE4B4-391E-474A-9621-08E11B188749}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3596,17 +3609,21 @@
       <c r="G2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="H2" s="22"/>
+      <c r="H2" s="22" t="s">
+        <v>124</v>
+      </c>
       <c r="I2" s="22" t="s">
-        <v>37</v>
+        <v>510</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" s="22"/>
+        <v>511</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>512</v>
+      </c>
       <c r="L2" s="22"/>
       <c r="M2" s="22" t="s">
-        <v>113</v>
+        <v>513</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -3616,7 +3633,7 @@
       <c r="B3" s="52"/>
       <c r="C3" s="52"/>
       <c r="D3" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="22" t="s">
@@ -3629,13 +3646,13 @@
         <v>86</v>
       </c>
       <c r="I3" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="J3" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="M3" s="22" t="s">
         <v>116</v>
-      </c>
-      <c r="M3" s="22" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -3645,7 +3662,7 @@
       <c r="B4" s="52"/>
       <c r="C4" s="52"/>
       <c r="D4" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E4" s="22"/>
       <c r="F4" s="22" t="s">
@@ -3658,13 +3675,13 @@
         <v>86</v>
       </c>
       <c r="I4" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="J4" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="J4" s="22" t="s">
-        <v>116</v>
-      </c>
       <c r="M4" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -3674,7 +3691,7 @@
       <c r="B5" s="52"/>
       <c r="C5" s="52"/>
       <c r="D5" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" s="22"/>
       <c r="F5" s="22" t="s">
@@ -3687,13 +3704,13 @@
         <v>86</v>
       </c>
       <c r="I5" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="J5" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="J5" s="22" t="s">
-        <v>116</v>
-      </c>
       <c r="M5" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -3702,32 +3719,32 @@
       </c>
       <c r="B6" s="52"/>
       <c r="C6" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="22" t="s">
         <v>122</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>123</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G6" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="H6" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="I6" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="J6" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="J6" s="22" t="s">
+      <c r="K6" t="s">
         <v>127</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" s="22" t="s">
         <v>128</v>
-      </c>
-      <c r="M6" s="22" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -3737,29 +3754,29 @@
       <c r="B7" s="52"/>
       <c r="C7" s="52"/>
       <c r="D7" s="22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G7" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="I7" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="J7" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="K7" t="s">
         <v>127</v>
       </c>
-      <c r="K7" t="s">
-        <v>128</v>
-      </c>
       <c r="M7" s="22" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -3769,29 +3786,29 @@
       <c r="B8" s="52"/>
       <c r="C8" s="52"/>
       <c r="D8" s="22" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" s="22" t="s">
         <v>124</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="I8" s="22" t="s">
         <v>125</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="J8" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="J8" s="22" t="s">
+      <c r="K8" t="s">
         <v>127</v>
       </c>
-      <c r="K8" t="s">
-        <v>128</v>
-      </c>
       <c r="M8" s="22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -3800,10 +3817,10 @@
       </c>
       <c r="B9" s="52"/>
       <c r="C9" s="52" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="22" t="s">
         <v>134</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>135</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="22" t="s">
@@ -3813,18 +3830,18 @@
         <v>17</v>
       </c>
       <c r="H9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I9" s="22"/>
       <c r="J9" s="22" t="s">
         <v>19</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L9" s="22"/>
       <c r="M9" s="22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -3834,7 +3851,7 @@
       <c r="B10" s="52"/>
       <c r="C10" s="52"/>
       <c r="D10" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="22" t="s">
@@ -3844,18 +3861,18 @@
         <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I10" s="22"/>
       <c r="J10" s="22" t="s">
         <v>19</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L10" s="22"/>
       <c r="M10" s="22" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -3865,7 +3882,7 @@
       <c r="B11" s="52"/>
       <c r="C11" s="52"/>
       <c r="D11" s="22" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22" t="s">
@@ -3875,18 +3892,18 @@
         <v>17</v>
       </c>
       <c r="H11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I11" s="22"/>
       <c r="J11" s="22" t="s">
         <v>19</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L11" s="22"/>
       <c r="M11" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -3896,7 +3913,7 @@
       <c r="B12" s="52"/>
       <c r="C12" s="52"/>
       <c r="D12" s="22" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="22" t="s">
@@ -3906,18 +3923,18 @@
         <v>17</v>
       </c>
       <c r="H12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="I12" s="22"/>
       <c r="J12" s="22" t="s">
         <v>19</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L12" s="22"/>
       <c r="M12" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -3925,10 +3942,10 @@
         <v>59</v>
       </c>
       <c r="B13" s="52" t="s">
+        <v>144</v>
+      </c>
+      <c r="C13" s="35" t="s">
         <v>145</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>146</v>
       </c>
       <c r="D13" s="25" t="s">
         <v>59</v>
@@ -3940,7 +3957,7 @@
       <c r="I13" s="20"/>
       <c r="J13" s="34"/>
       <c r="K13" s="34" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L13" s="34"/>
       <c r="M13" s="34"/>
@@ -3951,33 +3968,33 @@
       </c>
       <c r="B14" s="52"/>
       <c r="C14" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="22" t="s">
         <v>148</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>149</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H14" s="22" t="s">
         <v>36</v>
       </c>
       <c r="I14" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="J14" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="J14" s="22" t="s">
-        <v>127</v>
-      </c>
       <c r="K14" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L14" s="22"/>
       <c r="M14" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -3987,30 +4004,30 @@
       <c r="B15" s="52"/>
       <c r="C15" s="52"/>
       <c r="D15" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G15" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H15" s="22" t="s">
         <v>36</v>
       </c>
       <c r="I15" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="J15" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="J15" s="22" t="s">
-        <v>127</v>
-      </c>
       <c r="K15" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L15" s="22"/>
       <c r="M15" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -4020,30 +4037,30 @@
       <c r="B16" s="52"/>
       <c r="C16" s="52"/>
       <c r="D16" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E16" s="22"/>
       <c r="F16" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H16" s="22" t="s">
         <v>36</v>
       </c>
       <c r="I16" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="J16" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="J16" s="22" t="s">
-        <v>127</v>
-      </c>
       <c r="K16" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L16" s="22"/>
       <c r="M16" s="22" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -4053,30 +4070,30 @@
       <c r="B17" s="52"/>
       <c r="C17" s="52"/>
       <c r="D17" s="22" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H17" s="22" t="s">
         <v>36</v>
       </c>
       <c r="I17" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="J17" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="J17" s="22" t="s">
-        <v>127</v>
-      </c>
       <c r="K17" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L17" s="22"/>
       <c r="M17" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -4086,30 +4103,30 @@
       <c r="B18" s="52"/>
       <c r="C18" s="52"/>
       <c r="D18" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G18" s="22" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H18" s="22" t="s">
         <v>36</v>
       </c>
       <c r="I18" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="J18" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="J18" s="22" t="s">
-        <v>127</v>
-      </c>
       <c r="K18" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L18" s="22"/>
       <c r="M18" s="22" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -4117,13 +4134,13 @@
         <v>2</v>
       </c>
       <c r="B19" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="C19" s="52" t="s">
         <v>160</v>
       </c>
-      <c r="C19" s="52" t="s">
+      <c r="D19" s="22" t="s">
         <v>161</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>162</v>
       </c>
       <c r="E19" s="22"/>
       <c r="G19" s="22" t="s">
@@ -4133,17 +4150,17 @@
         <v>36</v>
       </c>
       <c r="I19" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="J19" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="J19" s="22" t="s">
+      <c r="K19" s="22" t="s">
         <v>164</v>
-      </c>
-      <c r="K19" s="22" t="s">
-        <v>165</v>
       </c>
       <c r="L19" s="22"/>
       <c r="M19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -4153,7 +4170,7 @@
       <c r="B20" s="52"/>
       <c r="C20" s="52"/>
       <c r="D20" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E20" s="22"/>
       <c r="G20" s="22" t="s">
@@ -4163,17 +4180,17 @@
         <v>36</v>
       </c>
       <c r="I20" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="J20" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="J20" s="22" t="s">
+      <c r="K20" s="22" t="s">
         <v>164</v>
-      </c>
-      <c r="K20" s="22" t="s">
-        <v>165</v>
       </c>
       <c r="L20" s="22"/>
       <c r="M20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -4183,7 +4200,7 @@
       <c r="B21" s="52"/>
       <c r="C21" s="52"/>
       <c r="D21" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E21" s="22"/>
       <c r="G21" s="22" t="s">
@@ -4193,17 +4210,17 @@
         <v>36</v>
       </c>
       <c r="I21" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="J21" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="J21" s="22" t="s">
+      <c r="K21" s="22" t="s">
         <v>164</v>
-      </c>
-      <c r="K21" s="22" t="s">
-        <v>165</v>
       </c>
       <c r="L21" s="22"/>
       <c r="M21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -4213,7 +4230,7 @@
       <c r="B22" s="52"/>
       <c r="C22" s="52"/>
       <c r="D22" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E22" s="22"/>
       <c r="G22" s="22" t="s">
@@ -4223,17 +4240,17 @@
         <v>36</v>
       </c>
       <c r="I22" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="J22" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="J22" s="22" t="s">
+      <c r="K22" s="22" t="s">
         <v>164</v>
-      </c>
-      <c r="K22" s="22" t="s">
-        <v>165</v>
       </c>
       <c r="L22" s="22"/>
       <c r="M22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -4243,7 +4260,7 @@
       <c r="B23" s="52"/>
       <c r="C23" s="52"/>
       <c r="D23" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E23" s="22"/>
       <c r="G23" s="22" t="s">
@@ -4251,17 +4268,17 @@
       </c>
       <c r="H23" s="22"/>
       <c r="I23" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="J23" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="J23" s="22" t="s">
+      <c r="K23" s="22" t="s">
         <v>164</v>
-      </c>
-      <c r="K23" s="22" t="s">
-        <v>165</v>
       </c>
       <c r="L23" s="22"/>
       <c r="M23" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -4271,7 +4288,7 @@
       <c r="B24" s="52"/>
       <c r="C24" s="52"/>
       <c r="D24" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
@@ -4280,17 +4297,17 @@
       </c>
       <c r="H24" s="22"/>
       <c r="I24" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="J24" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="J24" s="22" t="s">
+      <c r="K24" s="22" t="s">
         <v>164</v>
-      </c>
-      <c r="K24" s="22" t="s">
-        <v>165</v>
       </c>
       <c r="L24" s="22"/>
       <c r="M24" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -4300,7 +4317,7 @@
       <c r="B25" s="52"/>
       <c r="C25" s="52"/>
       <c r="D25" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
@@ -4309,17 +4326,17 @@
       </c>
       <c r="H25" s="22"/>
       <c r="I25" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="J25" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="J25" s="22" t="s">
+      <c r="K25" s="22" t="s">
         <v>164</v>
-      </c>
-      <c r="K25" s="22" t="s">
-        <v>165</v>
       </c>
       <c r="L25" s="22"/>
       <c r="M25" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -4329,7 +4346,7 @@
       <c r="B26" s="52"/>
       <c r="C26" s="52"/>
       <c r="D26" s="22" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
@@ -4338,17 +4355,17 @@
       </c>
       <c r="H26" s="22"/>
       <c r="I26" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="J26" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="J26" s="22" t="s">
+      <c r="K26" s="22" t="s">
         <v>164</v>
-      </c>
-      <c r="K26" s="22" t="s">
-        <v>165</v>
       </c>
       <c r="L26" s="22"/>
       <c r="M26" s="22" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -4357,14 +4374,14 @@
       </c>
       <c r="B27" s="52"/>
       <c r="C27" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="D27" s="22" t="s">
         <v>181</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>182</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G27" s="22" t="s">
         <v>35</v>
@@ -4373,13 +4390,13 @@
         <v>36</v>
       </c>
       <c r="I27" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="J27" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="J27" s="22" t="s">
+      <c r="K27" s="22" t="s">
         <v>185</v>
-      </c>
-      <c r="K27" s="22" t="s">
-        <v>507</v>
       </c>
       <c r="L27" s="22"/>
       <c r="M27" s="22" t="s">
@@ -4408,10 +4425,10 @@
         <v>36</v>
       </c>
       <c r="I28" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="J28" s="22" t="s">
         <v>163</v>
-      </c>
-      <c r="J28" s="22" t="s">
-        <v>164</v>
       </c>
       <c r="K28" s="22" t="s">
         <v>189</v>
@@ -4425,12 +4442,14 @@
       <c r="A29" s="26">
         <v>1</v>
       </c>
-      <c r="B29" s="52"/>
+      <c r="B29" s="52" t="s">
+        <v>509</v>
+      </c>
       <c r="C29" s="52" t="s">
         <v>191</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E29" s="22"/>
       <c r="F29" s="22" t="s">
@@ -4441,17 +4460,17 @@
       </c>
       <c r="H29" s="22"/>
       <c r="I29" s="22" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J29" s="22" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K29" s="22" t="s">
-        <v>508</v>
+        <v>195</v>
       </c>
       <c r="L29" s="22"/>
       <c r="M29" s="22" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -4461,7 +4480,7 @@
       <c r="B30" s="52"/>
       <c r="C30" s="52"/>
       <c r="D30" s="22" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E30" s="22"/>
       <c r="F30" s="22" t="s">
@@ -4472,17 +4491,17 @@
       </c>
       <c r="H30" s="22"/>
       <c r="I30" s="22" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J30" s="22" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K30" s="22" t="s">
-        <v>508</v>
+        <v>195</v>
       </c>
       <c r="L30" s="22"/>
       <c r="M30" s="22" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -4492,7 +4511,7 @@
       <c r="B31" s="52"/>
       <c r="C31" s="52"/>
       <c r="D31" s="22" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E31" s="22"/>
       <c r="F31" s="22" t="s">
@@ -4503,17 +4522,17 @@
       </c>
       <c r="H31" s="22"/>
       <c r="I31" s="22" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="J31" s="22" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="K31" s="22" t="s">
-        <v>508</v>
+        <v>195</v>
       </c>
       <c r="L31" s="22"/>
       <c r="M31" s="22" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -4522,29 +4541,29 @@
       </c>
       <c r="B32" s="52"/>
       <c r="C32" s="52" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D32" s="22" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E32" s="22"/>
       <c r="F32" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G32" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="H32" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="I32" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="J32" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="K32" s="22" t="s">
         <v>206</v>
-      </c>
-      <c r="H32" s="22" t="s">
-        <v>125</v>
-      </c>
-      <c r="I32" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="J32" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="K32" s="22" t="s">
-        <v>506</v>
       </c>
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
@@ -4556,30 +4575,30 @@
       <c r="B33" s="52"/>
       <c r="C33" s="52"/>
       <c r="D33" s="22" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E33" s="22"/>
       <c r="F33" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G33" s="22" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="H33" s="22" t="s">
         <v>36</v>
       </c>
       <c r="I33" s="22" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="J33" s="22" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="K33" s="22" t="s">
-        <v>505</v>
+        <v>211</v>
       </c>
       <c r="L33" s="22"/>
       <c r="M33" s="22" t="s">
-        <v>509</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
@@ -4587,32 +4606,32 @@
         <v>2</v>
       </c>
       <c r="B34" s="53" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="E34" s="22"/>
       <c r="F34" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="G34" s="22" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="H34" s="22" t="s">
         <v>26</v>
       </c>
       <c r="I34" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="J34" s="50" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="K34" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
@@ -4621,29 +4640,29 @@
       </c>
       <c r="B35" s="53"/>
       <c r="C35" s="53" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="D35" s="22" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="E35" s="22"/>
       <c r="F35" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="G35" s="22" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="H35" s="22" t="s">
         <v>26</v>
       </c>
       <c r="I35" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="J35" s="50" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="K35" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
@@ -4653,26 +4672,26 @@
       <c r="B36" s="53"/>
       <c r="C36" s="53"/>
       <c r="D36" s="22" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="E36" s="22"/>
       <c r="F36" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="G36" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="H36" s="22" t="s">
         <v>26</v>
       </c>
       <c r="I36" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="J36" s="50" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="K36" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
@@ -4682,26 +4701,26 @@
       <c r="B37" s="53"/>
       <c r="C37" s="53"/>
       <c r="D37" s="22" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="E37" s="22"/>
       <c r="F37" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="G37" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="H37" s="22" t="s">
         <v>26</v>
       </c>
       <c r="I37" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="J37" s="50" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="K37" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
@@ -4710,29 +4729,29 @@
       </c>
       <c r="B38" s="53"/>
       <c r="C38" s="53" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="D38" s="22" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="E38" s="22"/>
       <c r="F38" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="G38" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="H38" s="22" t="s">
         <v>26</v>
       </c>
       <c r="I38" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="J38" s="50" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="K38" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
@@ -4742,26 +4761,26 @@
       <c r="B39" s="53"/>
       <c r="C39" s="53"/>
       <c r="D39" s="22" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="E39" s="22"/>
       <c r="F39" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="G39" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="H39" s="22" t="s">
         <v>26</v>
       </c>
       <c r="I39" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="J39" s="50" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="K39" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -4801,8 +4820,8 @@
   <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4862,13 +4881,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22" t="s">
@@ -4881,17 +4900,17 @@
         <v>36</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="J2" s="22" t="s">
         <v>43</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="L2" s="22"/>
       <c r="M2" s="22" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -4901,7 +4920,7 @@
       <c r="B3" s="52"/>
       <c r="C3" s="52"/>
       <c r="D3" s="22" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="22" t="s">
@@ -4914,17 +4933,17 @@
         <v>36</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="J3" s="22" t="s">
         <v>43</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="L3" s="22"/>
       <c r="M3" s="22" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -4932,36 +4951,36 @@
         <v>2</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="E4" s="22"/>
       <c r="F4" s="22" t="s">
         <v>85</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
       <c r="L4" s="22"/>
       <c r="M4" s="22" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -4970,7 +4989,7 @@
       </c>
       <c r="B5" s="52"/>
       <c r="C5" s="42" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="D5" s="43" t="s">
         <v>59</v>
@@ -4982,7 +5001,7 @@
       <c r="I5" s="34"/>
       <c r="J5" s="34"/>
       <c r="K5" s="34" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="L5" s="34"/>
       <c r="M5" s="25" t="s">
@@ -4995,10 +5014,10 @@
       </c>
       <c r="B6" s="52"/>
       <c r="C6" s="52" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="22" t="s">
@@ -5011,17 +5030,17 @@
         <v>36</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="L6" s="22"/>
       <c r="M6" s="22" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -5031,7 +5050,7 @@
       <c r="B7" s="52"/>
       <c r="C7" s="52"/>
       <c r="D7" s="22" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="22" t="s">
@@ -5048,11 +5067,11 @@
         <v>38</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="L7" s="22"/>
       <c r="M7" s="22" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -5062,30 +5081,30 @@
       <c r="B8" s="52"/>
       <c r="C8" s="52"/>
       <c r="D8" s="22" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22" t="s">
         <v>85</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="H8" s="22" t="s">
         <v>36</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="L8" s="22"/>
       <c r="M8" s="22" t="s">
-        <v>251</v>
+        <v>255</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -5095,30 +5114,30 @@
       <c r="B9" s="52"/>
       <c r="C9" s="52"/>
       <c r="D9" s="22" t="s">
-        <v>252</v>
+        <v>256</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="22" t="s">
         <v>85</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="L9" s="22"/>
       <c r="M9" s="22" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -5128,30 +5147,30 @@
       <c r="B10" s="52"/>
       <c r="C10" s="52"/>
       <c r="D10" s="22" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="22" t="s">
         <v>85</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="I10" s="22" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="J10" s="22" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="K10" s="22" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="L10" s="22"/>
       <c r="M10" s="22" t="s">
-        <v>255</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -5160,10 +5179,10 @@
       </c>
       <c r="B11" s="52"/>
       <c r="C11" s="39" t="s">
-        <v>256</v>
+        <v>260</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22" t="s">
@@ -5176,17 +5195,17 @@
         <v>36</v>
       </c>
       <c r="I11" s="22" t="s">
-        <v>258</v>
+        <v>262</v>
       </c>
       <c r="J11" s="22" t="s">
-        <v>259</v>
+        <v>263</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="L11" s="22"/>
       <c r="M11" s="22" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -5195,7 +5214,7 @@
       </c>
       <c r="B12" s="52"/>
       <c r="C12" s="42" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="D12" s="43" t="s">
         <v>59</v>
@@ -5207,7 +5226,7 @@
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
       <c r="K12" s="34" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="L12" s="34"/>
       <c r="M12" s="25" t="s">
@@ -5220,10 +5239,10 @@
       </c>
       <c r="B13" s="52"/>
       <c r="C13" s="51" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="E13" s="22"/>
       <c r="F13" s="22" t="s">
@@ -5233,20 +5252,20 @@
         <v>35</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>267</v>
+        <v>271</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="L13" s="22"/>
       <c r="M13" s="22" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -5254,10 +5273,10 @@
         <v>59</v>
       </c>
       <c r="B14" s="53" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="D14" s="43" t="s">
         <v>59</v>
@@ -5280,7 +5299,7 @@
       </c>
       <c r="B15" s="53"/>
       <c r="C15" s="42" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
       <c r="D15" s="43" t="s">
         <v>59</v>
@@ -5292,7 +5311,7 @@
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
       <c r="K15" s="34" t="s">
-        <v>274</v>
+        <v>278</v>
       </c>
       <c r="L15" s="34"/>
       <c r="M15" s="25" t="s">
@@ -5305,7 +5324,7 @@
       </c>
       <c r="B16" s="53"/>
       <c r="C16" s="44" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="D16" s="43" t="s">
         <v>59</v>
@@ -5327,10 +5346,10 @@
         <v>59</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>276</v>
+        <v>280</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>277</v>
+        <v>281</v>
       </c>
       <c r="D17" s="43" t="s">
         <v>59</v>
@@ -5342,7 +5361,7 @@
       <c r="I17" s="34"/>
       <c r="J17" s="34"/>
       <c r="K17" s="34" t="s">
-        <v>278</v>
+        <v>282</v>
       </c>
       <c r="L17" s="34"/>
       <c r="M17" s="25" t="s">
@@ -5354,10 +5373,10 @@
         <v>59</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>279</v>
+        <v>283</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>280</v>
+        <v>284</v>
       </c>
       <c r="D18" s="43" t="s">
         <v>59</v>
@@ -5369,7 +5388,7 @@
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
       <c r="K18" s="20" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="L18" s="20"/>
       <c r="M18" s="25" t="s">
@@ -5382,7 +5401,7 @@
       </c>
       <c r="B19" s="52"/>
       <c r="C19" s="44" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="D19" s="43" t="s">
         <v>59</v>
@@ -5405,10 +5424,10 @@
       </c>
       <c r="B20" s="52"/>
       <c r="C20" s="53" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="22" t="s">
@@ -5425,11 +5444,11 @@
         <v>38</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="L20" s="22"/>
       <c r="M20" s="22" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -5439,7 +5458,7 @@
       <c r="B21" s="52"/>
       <c r="C21" s="53"/>
       <c r="D21" s="22" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="E21" s="22"/>
       <c r="F21" s="22" t="s">
@@ -5456,11 +5475,11 @@
         <v>38</v>
       </c>
       <c r="K21" s="22" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="L21" s="22"/>
       <c r="M21" s="22" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -5469,7 +5488,7 @@
       </c>
       <c r="B22" s="52"/>
       <c r="C22" s="44" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="D22" s="43" t="s">
         <v>59</v>
@@ -5481,7 +5500,7 @@
       <c r="I22" s="20"/>
       <c r="J22" s="20"/>
       <c r="K22" s="20" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="L22" s="20"/>
       <c r="M22" s="25" t="s">
@@ -5493,13 +5512,13 @@
         <v>3</v>
       </c>
       <c r="B23" s="52" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="C23" s="39" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="E23" s="22"/>
       <c r="F23" s="22" t="s">
@@ -5509,7 +5528,7 @@
         <v>35</v>
       </c>
       <c r="H23" s="22" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="I23" s="22" t="s">
         <v>37</v>
@@ -5518,7 +5537,7 @@
         <v>38</v>
       </c>
       <c r="M23" s="22" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -5527,10 +5546,10 @@
       </c>
       <c r="B24" s="52"/>
       <c r="C24" s="52" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="E24" s="22"/>
       <c r="F24" s="22" t="s">
@@ -5540,19 +5559,19 @@
         <v>17</v>
       </c>
       <c r="H24" s="22" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="J24" s="22" t="s">
         <v>43</v>
       </c>
       <c r="K24" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="M24" s="22" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -5562,7 +5581,7 @@
       <c r="B25" s="52"/>
       <c r="C25" s="52"/>
       <c r="D25" s="22" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="E25" s="22"/>
       <c r="F25" s="22" t="s">
@@ -5572,10 +5591,10 @@
         <v>17</v>
       </c>
       <c r="H25" s="22" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="J25" s="22" t="s">
         <v>43</v>
@@ -5583,7 +5602,7 @@
       <c r="K25" s="22"/>
       <c r="L25" s="22"/>
       <c r="M25" s="22" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -5593,7 +5612,7 @@
       <c r="B26" s="52"/>
       <c r="C26" s="52"/>
       <c r="D26" s="22" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="22" t="s">
@@ -5604,17 +5623,17 @@
       </c>
       <c r="H26" s="22"/>
       <c r="I26" s="22" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="J26" s="22" t="s">
         <v>43</v>
       </c>
       <c r="K26" s="22" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="L26" s="22"/>
       <c r="M26" s="22" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -5623,10 +5642,10 @@
       </c>
       <c r="B27" s="52"/>
       <c r="C27" s="40" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22" t="s">
@@ -5643,11 +5662,11 @@
         <v>38</v>
       </c>
       <c r="K27" s="22" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
       <c r="L27" s="22"/>
       <c r="M27" s="22" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -5656,7 +5675,7 @@
       </c>
       <c r="B28" s="52"/>
       <c r="C28" s="42" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="D28" s="43" t="s">
         <v>59</v>
@@ -5679,10 +5698,10 @@
       </c>
       <c r="B29" s="52"/>
       <c r="C29" s="52" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="E29" s="22"/>
       <c r="F29" s="22" t="s">
@@ -5692,7 +5711,7 @@
         <v>35</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="I29" s="22" t="s">
         <v>37</v>
@@ -5703,7 +5722,7 @@
       <c r="K29" s="22"/>
       <c r="L29" s="22"/>
       <c r="M29" s="22" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -5713,7 +5732,7 @@
       <c r="B30" s="52"/>
       <c r="C30" s="52"/>
       <c r="D30" s="22" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="E30" s="22"/>
       <c r="F30" s="22" t="s">
@@ -5723,7 +5742,7 @@
         <v>35</v>
       </c>
       <c r="H30" s="22" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="I30" s="22" t="s">
         <v>37</v>
@@ -5732,11 +5751,11 @@
         <v>38</v>
       </c>
       <c r="K30" s="22" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="L30" s="22"/>
       <c r="M30" s="22" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -5746,7 +5765,7 @@
       <c r="B31" s="52"/>
       <c r="C31" s="52"/>
       <c r="D31" s="22" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="E31" s="22"/>
       <c r="F31" s="22" t="s">
@@ -5756,7 +5775,7 @@
         <v>35</v>
       </c>
       <c r="H31" s="22" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="I31" s="22" t="s">
         <v>37</v>
@@ -5767,7 +5786,7 @@
       <c r="K31" s="22"/>
       <c r="L31" s="22"/>
       <c r="M31" s="22" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -5777,7 +5796,7 @@
       <c r="B32" s="52"/>
       <c r="C32" s="52"/>
       <c r="D32" s="22" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="E32" s="22"/>
       <c r="F32" s="22" t="s">
@@ -5787,7 +5806,7 @@
         <v>35</v>
       </c>
       <c r="H32" s="22" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="I32" s="22" t="s">
         <v>37</v>
@@ -5798,7 +5817,7 @@
       <c r="K32" s="22"/>
       <c r="L32" s="22"/>
       <c r="M32" s="22" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
@@ -5807,7 +5826,7 @@
       </c>
       <c r="B33" s="52"/>
       <c r="C33" s="38" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="D33" s="43" t="s">
         <v>59</v>
@@ -5818,7 +5837,9 @@
       <c r="H33" s="20"/>
       <c r="I33" s="20"/>
       <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
+      <c r="K33" s="20" t="s">
+        <v>508</v>
+      </c>
       <c r="L33" s="20"/>
       <c r="M33" s="25" t="s">
         <v>59</v>
@@ -5829,10 +5850,10 @@
         <v>59</v>
       </c>
       <c r="B34" s="39" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="C34" s="42" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="D34" s="43" t="s">
         <v>59</v>
@@ -5879,7 +5900,7 @@
   <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5944,13 +5965,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22" t="s">
@@ -5963,17 +5984,17 @@
         <v>86</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="L2" s="22"/>
       <c r="M2" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -5982,10 +6003,10 @@
       </c>
       <c r="B3" s="54"/>
       <c r="C3" s="28" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="22" t="s">
@@ -5998,16 +6019,16 @@
         <v>86</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="K3" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="M3" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
@@ -6015,10 +6036,10 @@
         <v>59</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="D4" s="34" t="s">
         <v>59</v>
@@ -6030,7 +6051,7 @@
       <c r="I4" s="34"/>
       <c r="J4" s="34"/>
       <c r="K4" s="34" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="L4" s="34"/>
     </row>
@@ -6040,7 +6061,7 @@
       </c>
       <c r="B5" s="55"/>
       <c r="C5" s="35" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="D5" s="34" t="s">
         <v>59</v>
@@ -6060,7 +6081,7 @@
       </c>
       <c r="B6" s="55"/>
       <c r="C6" s="35" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="D6" s="34" t="s">
         <v>59</v>
@@ -6072,7 +6093,7 @@
       <c r="I6" s="34"/>
       <c r="J6" s="34"/>
       <c r="K6" s="34" t="s">
-        <v>504</v>
+        <v>343</v>
       </c>
       <c r="L6" s="34"/>
     </row>
@@ -6082,7 +6103,7 @@
       </c>
       <c r="B7" s="55"/>
       <c r="C7" s="35" t="s">
-        <v>339</v>
+        <v>344</v>
       </c>
       <c r="D7" s="34" t="s">
         <v>59</v>
@@ -6094,7 +6115,7 @@
       <c r="I7" s="34"/>
       <c r="J7" s="34"/>
       <c r="K7" s="34" t="s">
-        <v>504</v>
+        <v>343</v>
       </c>
       <c r="L7" s="34"/>
     </row>
@@ -6103,17 +6124,17 @@
         <v>2</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>340</v>
+        <v>345</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>341</v>
+        <v>346</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>35</v>
@@ -6122,17 +6143,17 @@
         <v>26</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>343</v>
+        <v>348</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>345</v>
+        <v>350</v>
       </c>
       <c r="L8" s="22"/>
       <c r="M8" t="s">
-        <v>346</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
@@ -6140,10 +6161,10 @@
         <v>59</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>347</v>
+        <v>352</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
       <c r="D9" s="34" t="s">
         <v>59</v>
@@ -6155,7 +6176,7 @@
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
       <c r="K9" s="34" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
       <c r="L9" s="34"/>
     </row>
@@ -6164,13 +6185,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="30" t="s">
@@ -6191,7 +6212,7 @@
       <c r="K10" s="30"/>
       <c r="L10" s="30"/>
       <c r="M10" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -6199,13 +6220,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22" t="s">
@@ -6224,10 +6245,10 @@
         <v>20</v>
       </c>
       <c r="K11" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="M11" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -6236,10 +6257,10 @@
       </c>
       <c r="B12" s="52"/>
       <c r="C12" s="28" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="22" t="s">
@@ -6260,14 +6281,14 @@
       <c r="K12" s="22"/>
       <c r="L12" s="22"/>
       <c r="M12" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="26"/>
       <c r="B13" s="52"/>
       <c r="C13" s="42" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
       <c r="D13" s="34" t="s">
         <v>59</v>
@@ -6279,7 +6300,7 @@
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
       <c r="K13" s="34" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="L13" s="34"/>
       <c r="M13" s="34"/>
@@ -6290,10 +6311,10 @@
       </c>
       <c r="B14" s="52"/>
       <c r="C14" s="52" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="22" t="s">
@@ -6303,7 +6324,7 @@
         <v>17</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="I14" s="22" t="s">
         <v>76</v>
@@ -6314,7 +6335,7 @@
       <c r="K14" s="22"/>
       <c r="L14" s="22"/>
       <c r="M14" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -6324,7 +6345,7 @@
       <c r="B15" s="52"/>
       <c r="C15" s="52"/>
       <c r="D15" s="22" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="22" t="s">
@@ -6334,7 +6355,7 @@
         <v>17</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="I15" s="22" t="s">
         <v>76</v>
@@ -6345,7 +6366,7 @@
       <c r="K15" s="22"/>
       <c r="L15" s="22"/>
       <c r="M15" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
@@ -6354,7 +6375,7 @@
       </c>
       <c r="B16" s="52"/>
       <c r="C16" s="35" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="D16" s="34" t="s">
         <v>59</v>
@@ -6366,7 +6387,7 @@
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
       <c r="K16" s="34" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="L16" s="34"/>
     </row>
@@ -6375,10 +6396,10 @@
         <v>59</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="D17" s="48" t="s">
         <v>59</v>
@@ -6390,7 +6411,7 @@
       <c r="I17" s="35"/>
       <c r="J17" s="35"/>
       <c r="K17" s="48" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
       <c r="L17" s="35"/>
       <c r="M17" s="35"/>
@@ -6417,7 +6438,7 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D27" sqref="D27"/>
+      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6475,10 +6496,10 @@
         <v>59</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
       <c r="D2" t="s">
         <v>59</v>
@@ -6489,7 +6510,7 @@
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
       <c r="J2" s="20" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="K2" s="20"/>
       <c r="L2" s="20"/>
@@ -6500,7 +6521,7 @@
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="38" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="D3" t="s">
         <v>59</v>
@@ -6520,7 +6541,7 @@
       </c>
       <c r="B4" s="53"/>
       <c r="C4" s="38" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="D4" t="s">
         <v>59</v>
@@ -6540,7 +6561,7 @@
       </c>
       <c r="B5" s="53"/>
       <c r="C5" s="38" t="s">
-        <v>380</v>
+        <v>385</v>
       </c>
       <c r="D5" t="s">
         <v>59</v>
@@ -6560,10 +6581,10 @@
       </c>
       <c r="B6" s="53"/>
       <c r="C6" s="53" t="s">
-        <v>381</v>
+        <v>386</v>
       </c>
       <c r="D6" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
@@ -6572,7 +6593,7 @@
         <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H6" t="s">
         <v>37</v>
@@ -6581,11 +6602,11 @@
         <v>38</v>
       </c>
       <c r="J6" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="K6"/>
       <c r="L6" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6595,7 +6616,7 @@
       <c r="B7" s="53"/>
       <c r="C7" s="53"/>
       <c r="D7" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
@@ -6604,7 +6625,7 @@
         <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H7" t="s">
         <v>37</v>
@@ -6613,11 +6634,11 @@
         <v>38</v>
       </c>
       <c r="J7" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="K7"/>
       <c r="L7" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6626,7 +6647,7 @@
       </c>
       <c r="B8" s="53"/>
       <c r="C8" s="38" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="D8" t="s">
         <v>59</v>
@@ -6637,7 +6658,7 @@
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
       <c r="J8" s="20" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
@@ -6648,7 +6669,7 @@
       </c>
       <c r="B9" s="53"/>
       <c r="C9" s="38" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="D9" t="s">
         <v>59</v>
@@ -6659,7 +6680,7 @@
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
       <c r="J9" s="20" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
@@ -6669,13 +6690,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="53" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="D10" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
@@ -6684,7 +6705,7 @@
         <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H10" t="s">
         <v>19</v>
@@ -6693,11 +6714,11 @@
         <v>20</v>
       </c>
       <c r="J10" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="K10"/>
       <c r="L10" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6706,10 +6727,10 @@
       </c>
       <c r="B11" s="53"/>
       <c r="C11" s="29" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="D11" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="E11" t="s">
         <v>16</v>
@@ -6718,7 +6739,7 @@
         <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H11" t="s">
         <v>19</v>
@@ -6729,7 +6750,7 @@
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6738,10 +6759,10 @@
       </c>
       <c r="B12" s="53"/>
       <c r="C12" s="29" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="D12" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="E12" t="s">
         <v>16</v>
@@ -6750,7 +6771,7 @@
         <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H12" t="s">
         <v>19</v>
@@ -6761,7 +6782,7 @@
       <c r="J12"/>
       <c r="K12"/>
       <c r="L12" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6770,7 +6791,7 @@
       </c>
       <c r="B13" s="53"/>
       <c r="C13" s="38" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="D13" t="s">
         <v>59</v>
@@ -6781,7 +6802,7 @@
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
       <c r="J13" s="20" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
@@ -6791,10 +6812,10 @@
         <v>59</v>
       </c>
       <c r="B14" s="53" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="D14" s="41" t="s">
         <v>59</v>
@@ -6814,10 +6835,10 @@
       </c>
       <c r="B15" s="53"/>
       <c r="C15" s="53" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="D15" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="E15" t="s">
         <v>85</v>
@@ -6835,11 +6856,11 @@
         <v>20</v>
       </c>
       <c r="J15" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="K15"/>
       <c r="L15" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6849,7 +6870,7 @@
       <c r="B16" s="53"/>
       <c r="C16" s="53"/>
       <c r="D16" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="E16" t="s">
         <v>85</v>
@@ -6867,11 +6888,11 @@
         <v>20</v>
       </c>
       <c r="J16" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="K16"/>
       <c r="L16" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6881,7 +6902,7 @@
       <c r="B17" s="53"/>
       <c r="C17" s="53"/>
       <c r="D17" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="E17" t="s">
         <v>85</v>
@@ -6899,11 +6920,11 @@
         <v>20</v>
       </c>
       <c r="J17" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="K17"/>
       <c r="L17" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6912,7 +6933,7 @@
       </c>
       <c r="B18" s="53"/>
       <c r="C18" s="38" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>59</v>
@@ -6931,13 +6952,13 @@
         <v>1</v>
       </c>
       <c r="B19" s="53" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="C19" s="53" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="D19" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="E19" t="s">
         <v>16</v>
@@ -6946,7 +6967,7 @@
         <v>35</v>
       </c>
       <c r="G19" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H19" t="s">
         <v>37</v>
@@ -6957,7 +6978,7 @@
       <c r="J19"/>
       <c r="K19"/>
       <c r="L19" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6967,7 +6988,7 @@
       <c r="B20" s="53"/>
       <c r="C20" s="53"/>
       <c r="D20" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="E20" t="s">
         <v>16</v>
@@ -6976,7 +6997,7 @@
         <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H20" t="s">
         <v>37</v>
@@ -6987,7 +7008,7 @@
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6996,7 +7017,7 @@
       </c>
       <c r="B21" s="53"/>
       <c r="C21" s="38" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="D21" s="20" t="s">
         <v>59</v>
@@ -7007,7 +7028,7 @@
       <c r="H21" s="20"/>
       <c r="I21" s="20"/>
       <c r="J21" s="20" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
@@ -7018,7 +7039,7 @@
       </c>
       <c r="B22" s="53"/>
       <c r="C22" s="38" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>59</v>
@@ -7029,7 +7050,7 @@
       <c r="H22" s="20"/>
       <c r="I22" s="20"/>
       <c r="J22" s="20" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
@@ -7040,7 +7061,7 @@
       </c>
       <c r="B23" s="53"/>
       <c r="C23" s="38" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="D23" s="20" t="s">
         <v>59</v>
@@ -7051,7 +7072,7 @@
       <c r="H23" s="20"/>
       <c r="I23" s="20"/>
       <c r="J23" s="20" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
@@ -7062,7 +7083,7 @@
       </c>
       <c r="B24" s="53"/>
       <c r="C24" s="38" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="D24" s="20" t="s">
         <v>59</v>
@@ -7073,7 +7094,7 @@
       <c r="H24" s="20"/>
       <c r="I24" s="20"/>
       <c r="J24" s="20" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
@@ -7084,7 +7105,7 @@
       </c>
       <c r="B25" s="53"/>
       <c r="C25" s="38" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="D25" s="20" t="s">
         <v>59</v>
@@ -7095,7 +7116,7 @@
       <c r="H25" s="20"/>
       <c r="I25" s="20"/>
       <c r="J25" s="20" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="K25" s="20"/>
       <c r="L25" s="20"/>
@@ -7105,13 +7126,13 @@
         <v>1</v>
       </c>
       <c r="B26" s="53" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="C26" s="53" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="D26" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="E26" t="s">
         <v>16</v>
@@ -7120,7 +7141,7 @@
         <v>35</v>
       </c>
       <c r="G26" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H26" t="s">
         <v>37</v>
@@ -7129,11 +7150,11 @@
         <v>38</v>
       </c>
       <c r="J26" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="K26"/>
       <c r="L26" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -7143,7 +7164,7 @@
       <c r="B27" s="53"/>
       <c r="C27" s="53"/>
       <c r="D27" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="E27" t="s">
         <v>16</v>
@@ -7152,7 +7173,7 @@
         <v>35</v>
       </c>
       <c r="G27" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H27" t="s">
         <v>37</v>
@@ -7161,11 +7182,11 @@
         <v>38</v>
       </c>
       <c r="J27" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="K27"/>
       <c r="L27" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
     </row>
     <row r="28" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -7174,7 +7195,7 @@
       </c>
       <c r="B28" s="53"/>
       <c r="C28" s="38" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="D28" t="s">
         <v>59</v>
@@ -7194,7 +7215,7 @@
       </c>
       <c r="B29" s="53"/>
       <c r="C29" s="38" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="D29" t="s">
         <v>59</v>
@@ -7205,7 +7226,7 @@
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
       <c r="J29" s="20" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="K29" s="20"/>
       <c r="L29" s="20"/>
@@ -7216,15 +7237,15 @@
       </c>
       <c r="B30" s="53"/>
       <c r="C30" s="29" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="D30" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30" t="s">
-        <v>266</v>
+        <v>270</v>
       </c>
       <c r="H30" t="s">
         <v>42</v>
@@ -7233,11 +7254,11 @@
         <v>43</v>
       </c>
       <c r="J30" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="K30"/>
       <c r="L30" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -7324,18 +7345,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="58" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="B2" s="59"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="60" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="B3" s="61"/>
     </row>
@@ -7345,13 +7366,13 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="60" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="B5" s="61"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="56" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="B6" s="57"/>
     </row>
@@ -7361,13 +7382,13 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="60" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="B8" s="61"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="56" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="B9" s="57"/>
     </row>
@@ -7377,13 +7398,13 @@
     </row>
     <row r="11" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="64" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="B11" s="65"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="66" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="B12" s="61"/>
     </row>
@@ -7393,19 +7414,19 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="60" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="B14" s="61"/>
     </row>
     <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="62" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="B15" s="63"/>
     </row>
     <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="B17" s="2"/>
     </row>
@@ -7414,15 +7435,15 @@
         <v>11</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>455</v>
+        <v>459</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -7430,7 +7451,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -7438,7 +7459,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>457</v>
+        <v>461</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -7446,7 +7467,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>458</v>
+        <v>462</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -7454,7 +7475,7 @@
         <v>6</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -7462,15 +7483,15 @@
         <v>7</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>462</v>
+        <v>466</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -7478,23 +7499,23 @@
         <v>0</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>465</v>
+        <v>469</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
-        <v>466</v>
+        <v>470</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -7503,16 +7524,16 @@
     </row>
     <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
       <c r="B30" s="2"/>
     </row>
     <row r="31" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>470</v>
+        <v>474</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -7520,25 +7541,25 @@
         <v>59</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>471</v>
+        <v>475</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>472</v>
+        <v>476</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>473</v>
+        <v>477</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>474</v>
+        <v>478</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -7611,13 +7632,13 @@
         <v>6</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>475</v>
+        <v>479</v>
       </c>
       <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>464</v>
+        <v>468</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>8</v>
@@ -7631,7 +7652,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -7643,32 +7664,32 @@
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>477</v>
+        <v>481</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>478</v>
+        <v>482</v>
       </c>
       <c r="C3" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="J3" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>482</v>
+        <v>486</v>
       </c>
       <c r="C4" t="s">
-        <v>483</v>
+        <v>487</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -7677,10 +7698,10 @@
         <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>484</v>
+        <v>488</v>
       </c>
       <c r="J4" t="s">
-        <v>485</v>
+        <v>489</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -7688,7 +7709,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>486</v>
+        <v>490</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
@@ -7699,27 +7720,27 @@
     </row>
     <row r="6" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>487</v>
+        <v>491</v>
       </c>
       <c r="C6" t="s">
-        <v>488</v>
+        <v>492</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="J6" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="C7" t="s">
-        <v>490</v>
+        <v>494</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
@@ -7728,7 +7749,7 @@
         <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>491</v>
+        <v>495</v>
       </c>
       <c r="I7" t="s">
         <v>19</v>
@@ -7739,71 +7760,71 @@
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>492</v>
+        <v>496</v>
       </c>
       <c r="C8" t="s">
-        <v>493</v>
+        <v>497</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>480</v>
+        <v>484</v>
       </c>
       <c r="J8" t="s">
-        <v>481</v>
+        <v>485</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="B9" t="s">
-        <v>495</v>
+        <v>499</v>
       </c>
       <c r="H9" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="B10" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="H10" t="s">
-        <v>498</v>
+        <v>502</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="B11" t="s">
-        <v>499</v>
+        <v>503</v>
       </c>
       <c r="G11" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>501</v>
+        <v>505</v>
       </c>
       <c r="G12" t="s">
-        <v>500</v>
+        <v>504</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>494</v>
+        <v>498</v>
       </c>
       <c r="B13" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="G13" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaning up repo, adding fips key to zip files, editing readme
</commit_message>
<xml_diff>
--- a/2_clean/secondary_metrics.xlsx
+++ b/2_clean/secondary_metrics.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdonov12\OneDrive - University of Vermont\Food Systems Research Center\Sustainability Metrics\Sustainability Metrics Manuscript\Metrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvmoffice-my.sharepoint.com/personal/swalshda_uvm_edu/Documents/Food Systems Research Center/Sustainability Metrics/Sustainability Metrics Manuscript/Metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DF1908-CE30-4112-84EC-9B98DA2512CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{A8DF1908-CE30-4112-84EC-9B98DA2512CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{350D48EF-383E-453E-9B76-831A30264385}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1860" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Economics" sheetId="3" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="516">
   <si>
     <t>quality</t>
   </si>
@@ -1578,6 +1578,24 @@
   </si>
   <si>
     <t>https://cfpub.epa.gov/ghgdata/inventoryexplorer/</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>stalled</t>
+  </si>
+  <si>
+    <t>in progress, switching to forest carbon dataset (Chris)</t>
+  </si>
+  <si>
+    <t>need new dataset</t>
+  </si>
+  <si>
+    <t>to do - get PRISM or SPEI data</t>
+  </si>
+  <si>
+    <t>to do - get SSURGO or other dataset</t>
   </si>
 </sst>
 </file>
@@ -2019,12 +2037,18 @@
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -2033,12 +2057,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3477,8 +3495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802AE4B4-391E-474A-9621-08E11B188749}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3488,8 +3506,7 @@
     <col min="4" max="4" width="36.33203125" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
     <col min="11" max="11" width="69.6640625" customWidth="1"/>
-    <col min="12" max="12" width="10.6640625" customWidth="1"/>
-    <col min="13" max="13" width="28.109375" customWidth="1"/>
+    <col min="12" max="13" width="28.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -3565,7 +3582,9 @@
       <c r="K2" s="22" t="s">
         <v>508</v>
       </c>
-      <c r="L2" s="22"/>
+      <c r="L2" s="22" t="s">
+        <v>510</v>
+      </c>
       <c r="M2" s="22" t="s">
         <v>507</v>
       </c>
@@ -3595,6 +3614,9 @@
       <c r="J3" s="18" t="s">
         <v>509</v>
       </c>
+      <c r="L3" t="s">
+        <v>511</v>
+      </c>
       <c r="M3" s="22" t="s">
         <v>109</v>
       </c>
@@ -3624,6 +3646,9 @@
       <c r="J4" s="18" t="s">
         <v>509</v>
       </c>
+      <c r="L4" t="s">
+        <v>511</v>
+      </c>
       <c r="M4" s="22" t="s">
         <v>111</v>
       </c>
@@ -3653,6 +3678,9 @@
       <c r="J5" s="18" t="s">
         <v>509</v>
       </c>
+      <c r="L5" t="s">
+        <v>511</v>
+      </c>
       <c r="M5" s="22" t="s">
         <v>113</v>
       </c>
@@ -3686,6 +3714,9 @@
       </c>
       <c r="K6" t="s">
         <v>119</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>512</v>
       </c>
       <c r="M6" s="22" t="s">
         <v>120</v>
@@ -3719,6 +3750,9 @@
       <c r="K7" t="s">
         <v>119</v>
       </c>
+      <c r="L7" s="22" t="s">
+        <v>512</v>
+      </c>
       <c r="M7" s="22" t="s">
         <v>122</v>
       </c>
@@ -3751,6 +3785,9 @@
       <c r="K8" t="s">
         <v>119</v>
       </c>
+      <c r="L8" s="22" t="s">
+        <v>512</v>
+      </c>
       <c r="M8" s="22" t="s">
         <v>124</v>
       </c>
@@ -3783,7 +3820,9 @@
       <c r="K9" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="L9" s="22"/>
+      <c r="L9" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M9" s="22" t="s">
         <v>129</v>
       </c>
@@ -3814,7 +3853,9 @@
       <c r="K10" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="L10" s="22"/>
+      <c r="L10" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M10" s="22" t="s">
         <v>131</v>
       </c>
@@ -3845,7 +3886,9 @@
       <c r="K11" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="L11" s="22"/>
+      <c r="L11" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M11" s="22" t="s">
         <v>133</v>
       </c>
@@ -3876,7 +3919,9 @@
       <c r="K12" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="L12" s="22"/>
+      <c r="L12" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M12" s="22" t="s">
         <v>135</v>
       </c>
@@ -3903,7 +3948,9 @@
       <c r="K13" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="L13" s="34"/>
+      <c r="L13" s="34" t="s">
+        <v>512</v>
+      </c>
       <c r="M13" s="34"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -3936,7 +3983,9 @@
       <c r="K14" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="L14" s="22"/>
+      <c r="L14" s="22" t="s">
+        <v>512</v>
+      </c>
       <c r="M14" s="22" t="s">
         <v>142</v>
       </c>
@@ -3969,7 +4018,9 @@
       <c r="K15" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="L15" s="22"/>
+      <c r="L15" s="22" t="s">
+        <v>512</v>
+      </c>
       <c r="M15" s="22" t="s">
         <v>144</v>
       </c>
@@ -4002,7 +4053,9 @@
       <c r="K16" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="L16" s="22"/>
+      <c r="L16" s="22" t="s">
+        <v>512</v>
+      </c>
       <c r="M16" s="22" t="s">
         <v>146</v>
       </c>
@@ -4035,7 +4088,9 @@
       <c r="K17" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="L17" s="22"/>
+      <c r="L17" s="22" t="s">
+        <v>512</v>
+      </c>
       <c r="M17" s="22" t="s">
         <v>148</v>
       </c>
@@ -4068,7 +4123,9 @@
       <c r="K18" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="L18" s="22"/>
+      <c r="L18" s="22" t="s">
+        <v>512</v>
+      </c>
       <c r="M18" s="22" t="s">
         <v>150</v>
       </c>
@@ -4102,7 +4159,9 @@
       <c r="K19" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="L19" s="22"/>
+      <c r="L19" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M19" t="s">
         <v>157</v>
       </c>
@@ -4132,7 +4191,9 @@
       <c r="K20" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="L20" s="22"/>
+      <c r="L20" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M20" t="s">
         <v>159</v>
       </c>
@@ -4162,7 +4223,9 @@
       <c r="K21" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="L21" s="22"/>
+      <c r="L21" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M21" t="s">
         <v>161</v>
       </c>
@@ -4192,7 +4255,9 @@
       <c r="K22" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="L22" s="22"/>
+      <c r="L22" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M22" t="s">
         <v>163</v>
       </c>
@@ -4220,7 +4285,9 @@
       <c r="K23" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="L23" s="22"/>
+      <c r="L23" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M23" t="s">
         <v>165</v>
       </c>
@@ -4249,7 +4316,9 @@
       <c r="K24" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="L24" s="22"/>
+      <c r="L24" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M24" s="22" t="s">
         <v>167</v>
       </c>
@@ -4278,7 +4347,9 @@
       <c r="K25" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="L25" s="22"/>
+      <c r="L25" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M25" s="22" t="s">
         <v>169</v>
       </c>
@@ -4307,7 +4378,9 @@
       <c r="K26" s="22" t="s">
         <v>156</v>
       </c>
-      <c r="L26" s="22"/>
+      <c r="L26" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M26" s="22" t="s">
         <v>171</v>
       </c>
@@ -4342,7 +4415,9 @@
       <c r="K27" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="L27" s="22"/>
+      <c r="L27" s="22" t="s">
+        <v>510</v>
+      </c>
       <c r="M27" s="22" t="s">
         <v>178</v>
       </c>
@@ -4377,7 +4452,9 @@
       <c r="K28" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="L28" s="22"/>
+      <c r="L28" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M28" s="22" t="s">
         <v>182</v>
       </c>
@@ -4412,7 +4489,9 @@
       <c r="K29" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="L29" s="22"/>
+      <c r="L29" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M29" s="22" t="s">
         <v>189</v>
       </c>
@@ -4443,7 +4522,9 @@
       <c r="K30" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="L30" s="22"/>
+      <c r="L30" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M30" s="22" t="s">
         <v>191</v>
       </c>
@@ -4474,7 +4555,9 @@
       <c r="K31" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="L31" s="22"/>
+      <c r="L31" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M31" s="22" t="s">
         <v>193</v>
       </c>
@@ -4509,7 +4592,9 @@
       <c r="K32" s="22" t="s">
         <v>199</v>
       </c>
-      <c r="L32" s="22"/>
+      <c r="L32" s="22" t="s">
+        <v>514</v>
+      </c>
       <c r="M32" s="22"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
@@ -4540,7 +4625,9 @@
       <c r="K33" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="L33" s="22"/>
+      <c r="L33" s="22" t="s">
+        <v>510</v>
+      </c>
       <c r="M33" s="22" t="s">
         <v>205</v>
       </c>
@@ -4577,6 +4664,9 @@
       <c r="K34" t="s">
         <v>213</v>
       </c>
+      <c r="L34" s="22" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="23">
@@ -4607,6 +4697,9 @@
       </c>
       <c r="K35" t="s">
         <v>213</v>
+      </c>
+      <c r="L35" s="22" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
@@ -4637,6 +4730,9 @@
       <c r="K36" t="s">
         <v>213</v>
       </c>
+      <c r="L36" s="22" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="23">
@@ -4666,6 +4762,9 @@
       <c r="K37" t="s">
         <v>213</v>
       </c>
+      <c r="L37" s="22" t="s">
+        <v>515</v>
+      </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="23">
@@ -4696,6 +4795,9 @@
       </c>
       <c r="K38" t="s">
         <v>213</v>
+      </c>
+      <c r="L38" s="22" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
@@ -4725,6 +4827,9 @@
       </c>
       <c r="K39" t="s">
         <v>213</v>
+      </c>
+      <c r="L39" s="22" t="s">
+        <v>515</v>
       </c>
     </row>
   </sheetData>
@@ -5789,16 +5894,16 @@
     </sortState>
   </autoFilter>
   <mergeCells count="10">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B18:B22"/>
+    <mergeCell ref="B23:B32"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C6:C10"/>
     <mergeCell ref="C29:C31"/>
     <mergeCell ref="C24:C26"/>
     <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="B18:B22"/>
-    <mergeCell ref="B23:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7259,80 +7364,80 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="58" t="s">
         <v>436</v>
       </c>
-      <c r="B2" s="67"/>
+      <c r="B2" s="59"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="60" t="s">
         <v>437</v>
       </c>
-      <c r="B3" s="57"/>
+      <c r="B3" s="61"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="56"/>
-      <c r="B4" s="57"/>
+      <c r="A4" s="60"/>
+      <c r="B4" s="61"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="60" t="s">
         <v>438</v>
       </c>
-      <c r="B5" s="57"/>
+      <c r="B5" s="61"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="56" t="s">
         <v>439</v>
       </c>
-      <c r="B6" s="61"/>
+      <c r="B6" s="57"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="60"/>
-      <c r="B7" s="61"/>
+      <c r="A7" s="56"/>
+      <c r="B7" s="57"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="60" t="s">
         <v>440</v>
       </c>
-      <c r="B8" s="57"/>
+      <c r="B8" s="61"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="60" t="s">
+      <c r="A9" s="56" t="s">
         <v>441</v>
       </c>
-      <c r="B9" s="61"/>
+      <c r="B9" s="57"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="60"/>
-      <c r="B10" s="61"/>
+      <c r="A10" s="56"/>
+      <c r="B10" s="57"/>
     </row>
     <row r="11" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="64" t="s">
         <v>442</v>
       </c>
-      <c r="B11" s="63"/>
+      <c r="B11" s="65"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="66" t="s">
         <v>443</v>
       </c>
-      <c r="B12" s="57"/>
+      <c r="B12" s="61"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="65"/>
-      <c r="B13" s="57"/>
+      <c r="A13" s="67"/>
+      <c r="B13" s="61"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="56" t="s">
+      <c r="A14" s="60" t="s">
         <v>444</v>
       </c>
-      <c r="B14" s="57"/>
+      <c r="B14" s="61"/>
     </row>
     <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="62" t="s">
         <v>445</v>
       </c>
-      <c r="B15" s="59"/>
+      <c r="B15" s="63"/>
     </row>
     <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
@@ -7477,12 +7582,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A8:B8"/>
@@ -7491,6 +7590,12 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A9" r:id="rId1" xr:uid="{A59DB292-A126-46C8-AAB0-2FF5AD1DDD57}"/>

</xml_diff>

<commit_message>
reworking nass api parameters
</commit_message>
<xml_diff>
--- a/2_clean/secondary_metrics.xlsx
+++ b/2_clean/secondary_metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvmoffice-my.sharepoint.com/personal/swalshda_uvm_edu/Documents/Food Systems Research Center/Sustainability Metrics/Sustainability Metrics Manuscript/Metrics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{A8DF1908-CE30-4112-84EC-9B98DA2512CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{350D48EF-383E-453E-9B76-831A30264385}"/>
+  <xr:revisionPtr revIDLastSave="235" documentId="13_ncr:1_{A8DF1908-CE30-4112-84EC-9B98DA2512CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E680F50-79C8-4955-8B36-A7F59753DCF6}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1860" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="14592" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Economics" sheetId="3" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1291" uniqueCount="543">
   <si>
     <t>quality</t>
   </si>
@@ -392,12 +392,6 @@
     <t>N2OFromAg</t>
   </si>
   <si>
-    <t>above ground carbon stocks</t>
-  </si>
-  <si>
-    <t>Forest carbon - dead and down</t>
-  </si>
-  <si>
     <t>8 years</t>
   </si>
   <si>
@@ -407,24 +401,6 @@
     <t>https://data.fs.usda.gov/geodata/rastergateway/treemap/index.php</t>
   </si>
   <si>
-    <t>Slow (no) updates, and need more than just forests. Need a better source. Could try FEMC</t>
-  </si>
-  <si>
-    <t>forestCarbonDeadDown</t>
-  </si>
-  <si>
-    <t>Forest carbon - live standing</t>
-  </si>
-  <si>
-    <t>forestCarbonLive</t>
-  </si>
-  <si>
-    <t>Forest carbon - standing dead</t>
-  </si>
-  <si>
-    <t>forestCarbonDeadStanding</t>
-  </si>
-  <si>
     <t>embodied carbon</t>
   </si>
   <si>
@@ -464,9 +440,6 @@
     <t>forest complexity</t>
   </si>
   <si>
-    <t>TreeMap has some data, but old. FEMC is an option, but not great coverage</t>
-  </si>
-  <si>
     <t>forest health</t>
   </si>
   <si>
@@ -662,9 +635,6 @@
     <t>https://droughtmonitor.unl.edu/DmData/DataDownload.aspx</t>
   </si>
   <si>
-    <t>This is tabular pulled from API, but they also have rasters and vectors</t>
-  </si>
-  <si>
     <t>droughtNonConWeeksCat2</t>
   </si>
   <si>
@@ -1070,9 +1040,6 @@
     <t>https://www.nass.usda.gov/Research_and_Science/Cropland/SARS1a.php</t>
   </si>
   <si>
-    <t>Might not be great measure for NE states - could alternatively try it from NASS production stats</t>
-  </si>
-  <si>
     <t>cropDiversity</t>
   </si>
   <si>
@@ -1253,9 +1220,6 @@
     <t>Acres under conservation easements</t>
   </si>
   <si>
-    <t>state only, not available at county</t>
-  </si>
-  <si>
     <t>consEasementAcres</t>
   </si>
   <si>
@@ -1391,9 +1355,6 @@
     <t>Variables:</t>
   </si>
   <si>
-    <t>where we're at with data wrangling. Done = all ready to use. Rework = we have data, just need to transform it or do calculations. Find source = we want this but don't have it, and have no leads. Pull it = we have a source/lead, just have to pull and wrangle it</t>
-  </si>
-  <si>
     <t>dimension:metric</t>
   </si>
   <si>
@@ -1547,9 +1508,6 @@
     <t>Gender pay gap in agricultural sector</t>
   </si>
   <si>
-    <t>Proportion of womens' pay to mens' pay in agriculture sector (NAICS 11)</t>
-  </si>
-  <si>
     <t>Might like this better than general pay gap or income inequality. Could also consider sector 111? Maybe 112?</t>
   </si>
   <si>
@@ -1583,12 +1541,6 @@
     <t>done</t>
   </si>
   <si>
-    <t>stalled</t>
-  </si>
-  <si>
-    <t>in progress, switching to forest carbon dataset (Chris)</t>
-  </si>
-  <si>
     <t>need new dataset</t>
   </si>
   <si>
@@ -1596,6 +1548,135 @@
   </si>
   <si>
     <t>to do - get SSURGO or other dataset</t>
+  </si>
+  <si>
+    <t>to do - rework as distribution or diversity index</t>
+  </si>
+  <si>
+    <t>to do - calculate ratio</t>
+  </si>
+  <si>
+    <t>Ratio of womens' pay to mens' pay in agriculture sector (NAICS 11)</t>
+  </si>
+  <si>
+    <t>to do - wrangle this from NASS</t>
+  </si>
+  <si>
+    <t>in progress - switch these to NASS from FAME (Chris)</t>
+  </si>
+  <si>
+    <t>to do - get new dataset, leads from Gillian</t>
+  </si>
+  <si>
+    <t>done unless better dataset</t>
+  </si>
+  <si>
+    <t>in progress (Chris) - get this from source instead of FAME</t>
+  </si>
+  <si>
+    <t>done unless we want source rather than UW</t>
+  </si>
+  <si>
+    <t>done unless source rather than UW, but UW data looks cleaner than source</t>
+  </si>
+  <si>
+    <t>to do - pull from cdc eph or elsewhere. But eph data is very spotty.</t>
+  </si>
+  <si>
+    <t>in progress (Chris) - is this available at county level, or something similar?</t>
+  </si>
+  <si>
+    <t>in progress (Chris) - fix variable_name</t>
+  </si>
+  <si>
+    <t>in progress (Chris) - find this and fix name</t>
+  </si>
+  <si>
+    <t>need a plan here</t>
+  </si>
+  <si>
+    <t>done unless we want source instead of UW - but UW is cleaner</t>
+  </si>
+  <si>
+    <t>to do - calculate from NASS</t>
+  </si>
+  <si>
+    <t>in progress (Chris) - find this or calculate it again</t>
+  </si>
+  <si>
+    <t>to do - calculate Shannon from NASS</t>
+  </si>
+  <si>
+    <t>done unless we want source instead of UW</t>
+  </si>
+  <si>
+    <t>need dataset</t>
+  </si>
+  <si>
+    <t>done unless want source instead of UW</t>
+  </si>
+  <si>
+    <t>to do - calculate from census</t>
+  </si>
+  <si>
+    <t>carbon stocks</t>
+  </si>
+  <si>
+    <t>Aboveground biomass per acre</t>
+  </si>
+  <si>
+    <t>~10 years</t>
+  </si>
+  <si>
+    <t>USDA National Forest Carbon Monitoring System</t>
+  </si>
+  <si>
+    <t>https://www.fs.usda.gov/rds/archive/catalog/RDS-2025-0019</t>
+  </si>
+  <si>
+    <t>More recent data then TreeMap, but unclear on updates</t>
+  </si>
+  <si>
+    <t>Live biomass per acre</t>
+  </si>
+  <si>
+    <t>Soil carbon per acre</t>
+  </si>
+  <si>
+    <t>Total ecosystem carbon per acre</t>
+  </si>
+  <si>
+    <t>abovegroundBiomassPerAcre</t>
+  </si>
+  <si>
+    <t>liveBiomassPerAcre</t>
+  </si>
+  <si>
+    <t>soilCarbonPerAcre</t>
+  </si>
+  <si>
+    <t>totalEcosystemCarbonPerAcre</t>
+  </si>
+  <si>
+    <t>Forest type diversity</t>
+  </si>
+  <si>
+    <t>forestTypeDiversity</t>
+  </si>
+  <si>
+    <t>propForest</t>
+  </si>
+  <si>
+    <t>Proportion forested</t>
+  </si>
+  <si>
+    <t>where we're at with data wrangling</t>
+  </si>
+  <si>
+    <t>in progress (Chris) - switching to forest carbon dataset</t>
+  </si>
+  <si>
+    <t>This is tabular data pulled from API, but they also have rasters and vectors</t>
   </si>
 </sst>
 </file>
@@ -1906,7 +1987,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2057,6 +2138,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2526,8 +2610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0D1AE80-3BFB-3B41-8518-A67336181549}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2539,7 +2623,7 @@
     <col min="9" max="9" width="33.33203125" customWidth="1"/>
     <col min="10" max="10" width="10" customWidth="1"/>
     <col min="11" max="11" width="64.6640625" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" customWidth="1"/>
+    <col min="12" max="12" width="23.33203125" customWidth="1"/>
     <col min="13" max="13" width="36.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2614,7 +2698,9 @@
         <v>20</v>
       </c>
       <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
+      <c r="L2" s="22" t="s">
+        <v>496</v>
+      </c>
       <c r="M2" s="22" t="s">
         <v>21</v>
       </c>
@@ -2647,7 +2733,9 @@
       <c r="K3" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="22"/>
+      <c r="L3" s="22" t="s">
+        <v>496</v>
+      </c>
       <c r="M3" s="22" t="s">
         <v>24</v>
       </c>
@@ -2681,7 +2769,7 @@
         <v>27</v>
       </c>
       <c r="L4" s="22" t="s">
-        <v>28</v>
+        <v>500</v>
       </c>
       <c r="M4" s="22" t="s">
         <v>29</v>
@@ -2716,7 +2804,7 @@
         <v>27</v>
       </c>
       <c r="L5" s="22" t="s">
-        <v>28</v>
+        <v>500</v>
       </c>
       <c r="M5" s="22" t="s">
         <v>31</v>
@@ -2754,7 +2842,9 @@
       <c r="K6" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="L6" s="22"/>
+      <c r="L6" s="22" t="s">
+        <v>496</v>
+      </c>
       <c r="M6" s="22" t="s">
         <v>40</v>
       </c>
@@ -2787,7 +2877,9 @@
       <c r="K7" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="L7" s="22"/>
+      <c r="L7" s="22" t="s">
+        <v>496</v>
+      </c>
       <c r="M7" s="22" t="s">
         <v>45</v>
       </c>
@@ -2820,7 +2912,9 @@
       <c r="K8" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="L8" s="22"/>
+      <c r="L8" s="22" t="s">
+        <v>496</v>
+      </c>
       <c r="M8" s="22" t="s">
         <v>48</v>
       </c>
@@ -2830,20 +2924,32 @@
       <c r="B9" s="52"/>
       <c r="C9" s="53"/>
       <c r="D9" s="22" t="s">
-        <v>498</v>
+        <v>485</v>
       </c>
       <c r="E9" s="22" t="s">
-        <v>499</v>
-      </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
+        <v>502</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>253</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="22" t="s">
+        <v>20</v>
+      </c>
       <c r="K9" s="22" t="s">
-        <v>500</v>
-      </c>
-      <c r="L9" s="22"/>
+        <v>486</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>501</v>
+      </c>
       <c r="M9" s="22"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -2855,7 +2961,7 @@
         <v>49</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>506</v>
+        <v>492</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="22" t="s">
@@ -2874,9 +2980,11 @@
         <v>51</v>
       </c>
       <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
+      <c r="L10" s="22" t="s">
+        <v>496</v>
+      </c>
       <c r="M10" s="22" t="s">
-        <v>505</v>
+        <v>491</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -2936,7 +3044,9 @@
         <v>20</v>
       </c>
       <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
+      <c r="L12" s="22" t="s">
+        <v>503</v>
+      </c>
       <c r="M12" s="22"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -2965,7 +3075,9 @@
         <v>20</v>
       </c>
       <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
+      <c r="L13" s="22" t="s">
+        <v>496</v>
+      </c>
       <c r="M13" s="22" t="s">
         <v>61</v>
       </c>
@@ -2977,7 +3089,7 @@
       <c r="B14" s="52"/>
       <c r="C14" s="52"/>
       <c r="D14" s="22" t="s">
-        <v>503</v>
+        <v>489</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="22" t="s">
@@ -2996,9 +3108,11 @@
         <v>51</v>
       </c>
       <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
+      <c r="L14" s="22" t="s">
+        <v>496</v>
+      </c>
       <c r="M14" s="22" t="s">
-        <v>504</v>
+        <v>490</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -3079,7 +3193,9 @@
         <v>68</v>
       </c>
       <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
+      <c r="L17" s="22" t="s">
+        <v>504</v>
+      </c>
       <c r="M17" s="22" t="s">
         <v>69</v>
       </c>
@@ -3110,7 +3226,9 @@
         <v>68</v>
       </c>
       <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
+      <c r="L18" s="22" t="s">
+        <v>504</v>
+      </c>
       <c r="M18" s="22" t="s">
         <v>71</v>
       </c>
@@ -3141,7 +3259,9 @@
         <v>68</v>
       </c>
       <c r="K19" s="22"/>
-      <c r="L19" s="22"/>
+      <c r="L19" s="22" t="s">
+        <v>504</v>
+      </c>
       <c r="M19" s="22" t="s">
         <v>73</v>
       </c>
@@ -3176,7 +3296,9 @@
       <c r="K20" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="L20" s="22"/>
+      <c r="L20" s="22" t="s">
+        <v>505</v>
+      </c>
       <c r="M20" t="s">
         <v>81</v>
       </c>
@@ -3209,7 +3331,9 @@
       <c r="K21" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="L21" s="22"/>
+      <c r="L21" s="22" t="s">
+        <v>505</v>
+      </c>
       <c r="M21" t="s">
         <v>83</v>
       </c>
@@ -3242,7 +3366,9 @@
       <c r="K22" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="L22" s="22"/>
+      <c r="L22" s="22" t="s">
+        <v>505</v>
+      </c>
       <c r="M22" t="s">
         <v>85</v>
       </c>
@@ -3275,7 +3401,9 @@
       <c r="K23" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="L23" s="22"/>
+      <c r="L23" s="22" t="s">
+        <v>505</v>
+      </c>
       <c r="M23" t="s">
         <v>87</v>
       </c>
@@ -3308,7 +3436,9 @@
       <c r="K24" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="L24" s="22"/>
+      <c r="L24" s="22" t="s">
+        <v>505</v>
+      </c>
       <c r="M24" t="s">
         <v>89</v>
       </c>
@@ -3341,7 +3471,9 @@
       <c r="K25" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="L25" s="22"/>
+      <c r="L25" s="22" t="s">
+        <v>505</v>
+      </c>
       <c r="M25" t="s">
         <v>91</v>
       </c>
@@ -3374,7 +3506,9 @@
       <c r="K26" s="22" t="s">
         <v>80</v>
       </c>
-      <c r="L26" s="22"/>
+      <c r="L26" s="22" t="s">
+        <v>505</v>
+      </c>
       <c r="M26" t="s">
         <v>93</v>
       </c>
@@ -3493,10 +3627,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{802AE4B4-391E-474A-9621-08E11B188749}">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3580,13 +3714,13 @@
         <v>106</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>508</v>
+        <v>494</v>
       </c>
       <c r="L2" s="22" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="M2" s="22" t="s">
-        <v>507</v>
+        <v>493</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -3612,10 +3746,10 @@
         <v>108</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>509</v>
+        <v>495</v>
       </c>
       <c r="L3" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="M3" s="22" t="s">
         <v>109</v>
@@ -3644,10 +3778,10 @@
         <v>108</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>509</v>
+        <v>495</v>
       </c>
       <c r="L4" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="M4" s="22" t="s">
         <v>111</v>
@@ -3676,155 +3810,155 @@
         <v>108</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>509</v>
+        <v>495</v>
       </c>
       <c r="L5" t="s">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="M5" s="22" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="26">
-        <v>1</v>
+      <c r="A6" s="23">
+        <v>2</v>
       </c>
       <c r="B6" s="52"/>
       <c r="C6" s="52" t="s">
-        <v>114</v>
+        <v>523</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>115</v>
+        <v>524</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="22" t="s">
-        <v>16</v>
+        <v>165</v>
       </c>
       <c r="G6" s="22" t="s">
-        <v>116</v>
+        <v>525</v>
       </c>
       <c r="H6" s="22" t="s">
-        <v>104</v>
+        <v>36</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>117</v>
+        <v>526</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="K6" t="s">
-        <v>119</v>
+        <v>527</v>
+      </c>
+      <c r="K6" s="22" t="s">
+        <v>528</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>512</v>
+        <v>496</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>120</v>
+        <v>532</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="26">
-        <v>1</v>
+      <c r="A7" s="23">
+        <v>2</v>
       </c>
       <c r="B7" s="52"/>
       <c r="C7" s="52"/>
       <c r="D7" s="22" t="s">
-        <v>121</v>
+        <v>529</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="22" t="s">
-        <v>16</v>
+        <v>165</v>
       </c>
       <c r="G7" s="22" t="s">
-        <v>116</v>
+        <v>525</v>
       </c>
       <c r="H7" s="22" t="s">
-        <v>104</v>
+        <v>36</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>117</v>
+        <v>526</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="K7" t="s">
-        <v>119</v>
+        <v>527</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>528</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>512</v>
+        <v>496</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>122</v>
+        <v>533</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="26">
-        <v>1</v>
+      <c r="A8" s="23">
+        <v>2</v>
       </c>
       <c r="B8" s="52"/>
       <c r="C8" s="52"/>
       <c r="D8" s="22" t="s">
-        <v>123</v>
+        <v>530</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22" t="s">
-        <v>16</v>
+        <v>165</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>116</v>
+        <v>525</v>
       </c>
       <c r="H8" s="22" t="s">
-        <v>104</v>
+        <v>36</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>117</v>
+        <v>526</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="K8" t="s">
-        <v>119</v>
+        <v>527</v>
+      </c>
+      <c r="K8" s="22" t="s">
+        <v>528</v>
       </c>
       <c r="L8" s="22" t="s">
-        <v>512</v>
+        <v>496</v>
       </c>
       <c r="M8" s="22" t="s">
-        <v>124</v>
+        <v>534</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="26">
-        <v>1</v>
+      <c r="A9" s="23">
+        <v>2</v>
       </c>
       <c r="B9" s="52"/>
-      <c r="C9" s="52" t="s">
-        <v>125</v>
-      </c>
+      <c r="C9" s="52"/>
       <c r="D9" s="22" t="s">
-        <v>126</v>
+        <v>531</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="22" t="s">
-        <v>76</v>
+        <v>165</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" t="s">
-        <v>127</v>
+        <v>525</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>36</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="22"/>
+        <v>526</v>
+      </c>
+      <c r="J9" s="22" t="s">
+        <v>527</v>
+      </c>
       <c r="K9" s="22" t="s">
-        <v>128</v>
+        <v>528</v>
       </c>
       <c r="L9" s="22" t="s">
-        <v>513</v>
+        <v>496</v>
       </c>
       <c r="M9" s="22" t="s">
-        <v>129</v>
+        <v>535</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -3832,9 +3966,11 @@
         <v>1</v>
       </c>
       <c r="B10" s="52"/>
-      <c r="C10" s="52"/>
+      <c r="C10" s="52" t="s">
+        <v>117</v>
+      </c>
       <c r="D10" s="22" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="22" t="s">
@@ -3844,20 +3980,20 @@
         <v>17</v>
       </c>
       <c r="H10" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="I10" s="22" t="s">
         <v>19</v>
       </c>
       <c r="J10" s="22"/>
       <c r="K10" s="22" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="L10" s="22" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="M10" s="22" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -3867,7 +4003,7 @@
       <c r="B11" s="52"/>
       <c r="C11" s="52"/>
       <c r="D11" s="22" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22" t="s">
@@ -3877,20 +4013,20 @@
         <v>17</v>
       </c>
       <c r="H11" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="I11" s="22" t="s">
         <v>19</v>
       </c>
       <c r="J11" s="22"/>
       <c r="K11" s="22" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="L11" s="22" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="M11" s="22" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -3900,7 +4036,7 @@
       <c r="B12" s="52"/>
       <c r="C12" s="52"/>
       <c r="D12" s="22" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="22" t="s">
@@ -3910,84 +4046,92 @@
         <v>17</v>
       </c>
       <c r="H12" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="I12" s="22" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="22"/>
       <c r="K12" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>497</v>
+      </c>
+      <c r="M12" s="22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="26">
+        <v>1</v>
+      </c>
+      <c r="B13" s="52"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" t="s">
+        <v>119</v>
+      </c>
+      <c r="I13" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>497</v>
+      </c>
+      <c r="M13" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="23">
+        <v>2</v>
+      </c>
+      <c r="B14" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="L12" s="22" t="s">
-        <v>513</v>
-      </c>
-      <c r="M12" s="22" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="52" t="s">
-        <v>136</v>
-      </c>
-      <c r="C13" s="35" t="s">
-        <v>137</v>
-      </c>
-      <c r="D13" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34" t="s">
-        <v>138</v>
-      </c>
-      <c r="L13" s="34" t="s">
-        <v>512</v>
-      </c>
-      <c r="M13" s="34"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="26">
-        <v>1</v>
-      </c>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52" t="s">
-        <v>139</v>
+      <c r="C14" s="68" t="s">
+        <v>129</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>140</v>
+        <v>536</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="22" t="s">
-        <v>16</v>
+        <v>165</v>
       </c>
       <c r="G14" s="22" t="s">
-        <v>116</v>
+        <v>525</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>36</v>
+        <v>104</v>
       </c>
       <c r="I14" s="22" t="s">
-        <v>117</v>
+        <v>526</v>
       </c>
       <c r="J14" s="22" t="s">
-        <v>118</v>
+        <v>527</v>
       </c>
       <c r="K14" s="22" t="s">
-        <v>141</v>
+        <v>528</v>
       </c>
       <c r="L14" s="22" t="s">
-        <v>512</v>
+        <v>496</v>
       </c>
       <c r="M14" s="22" t="s">
-        <v>142</v>
+        <v>537</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -3995,34 +4139,36 @@
         <v>1</v>
       </c>
       <c r="B15" s="52"/>
-      <c r="C15" s="52"/>
+      <c r="C15" s="52" t="s">
+        <v>130</v>
+      </c>
       <c r="D15" s="22" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G15" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H15" s="22" t="s">
         <v>36</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J15" s="22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K15" s="22" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L15" s="22" t="s">
-        <v>512</v>
+        <v>541</v>
       </c>
       <c r="M15" s="22" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -4032,32 +4178,32 @@
       <c r="B16" s="52"/>
       <c r="C16" s="52"/>
       <c r="D16" s="22" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="E16" s="22"/>
       <c r="F16" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G16" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H16" s="22" t="s">
         <v>36</v>
       </c>
       <c r="I16" s="22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J16" s="22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K16" s="22" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L16" s="22" t="s">
-        <v>512</v>
+        <v>541</v>
       </c>
       <c r="M16" s="22" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -4067,32 +4213,32 @@
       <c r="B17" s="52"/>
       <c r="C17" s="52"/>
       <c r="D17" s="22" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G17" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H17" s="22" t="s">
         <v>36</v>
       </c>
       <c r="I17" s="22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J17" s="22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K17" s="22" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L17" s="22" t="s">
-        <v>512</v>
+        <v>541</v>
       </c>
       <c r="M17" s="22" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -4102,68 +4248,67 @@
       <c r="B18" s="52"/>
       <c r="C18" s="52"/>
       <c r="D18" s="22" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
       <c r="E18" s="22"/>
       <c r="F18" s="22" t="s">
         <v>16</v>
       </c>
       <c r="G18" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H18" s="22" t="s">
         <v>36</v>
       </c>
       <c r="I18" s="22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J18" s="22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K18" s="22" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="L18" s="22" t="s">
-        <v>512</v>
+        <v>541</v>
       </c>
       <c r="M18" s="22" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="23">
-        <v>2</v>
-      </c>
-      <c r="B19" s="52" t="s">
-        <v>151</v>
-      </c>
-      <c r="C19" s="52" t="s">
-        <v>152</v>
-      </c>
+      <c r="A19" s="26">
+        <v>1</v>
+      </c>
+      <c r="B19" s="52"/>
+      <c r="C19" s="52"/>
       <c r="D19" s="22" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="E19" s="22"/>
+      <c r="F19" s="22" t="s">
+        <v>16</v>
+      </c>
       <c r="G19" s="22" t="s">
-        <v>35</v>
+        <v>114</v>
       </c>
       <c r="H19" s="22" t="s">
         <v>36</v>
       </c>
       <c r="I19" s="22" t="s">
-        <v>154</v>
+        <v>115</v>
       </c>
       <c r="J19" s="22" t="s">
-        <v>155</v>
+        <v>116</v>
       </c>
       <c r="K19" s="22" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="L19" s="22" t="s">
-        <v>513</v>
-      </c>
-      <c r="M19" t="s">
-        <v>157</v>
+        <v>541</v>
+      </c>
+      <c r="M19" s="22" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
@@ -4173,41 +4318,51 @@
       <c r="B20" s="52"/>
       <c r="C20" s="52"/>
       <c r="D20" s="22" t="s">
-        <v>158</v>
+        <v>539</v>
       </c>
       <c r="E20" s="22"/>
+      <c r="F20" s="22" t="s">
+        <v>165</v>
+      </c>
       <c r="G20" s="22" t="s">
-        <v>35</v>
+        <v>525</v>
       </c>
       <c r="H20" s="22" t="s">
         <v>36</v>
       </c>
       <c r="I20" s="22" t="s">
-        <v>154</v>
+        <v>526</v>
       </c>
       <c r="J20" s="22" t="s">
-        <v>155</v>
+        <v>527</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>156</v>
+        <v>528</v>
       </c>
       <c r="L20" s="22" t="s">
-        <v>513</v>
-      </c>
-      <c r="M20" t="s">
-        <v>159</v>
+        <v>496</v>
+      </c>
+      <c r="M20" s="22" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="23">
         <v>2</v>
       </c>
-      <c r="B21" s="52"/>
-      <c r="C21" s="52"/>
+      <c r="B21" s="52" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" s="52" t="s">
+        <v>143</v>
+      </c>
       <c r="D21" s="22" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="E21" s="22"/>
+      <c r="F21" s="22" t="s">
+        <v>76</v>
+      </c>
       <c r="G21" s="22" t="s">
         <v>35</v>
       </c>
@@ -4215,19 +4370,19 @@
         <v>36</v>
       </c>
       <c r="I21" s="22" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="J21" s="22" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="K21" s="22" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="L21" s="22" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="M21" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -4237,9 +4392,12 @@
       <c r="B22" s="52"/>
       <c r="C22" s="52"/>
       <c r="D22" s="22" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="E22" s="22"/>
+      <c r="F22" s="22" t="s">
+        <v>76</v>
+      </c>
       <c r="G22" s="22" t="s">
         <v>35</v>
       </c>
@@ -4247,19 +4405,19 @@
         <v>36</v>
       </c>
       <c r="I22" s="22" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="J22" s="22" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="K22" s="22" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="L22" s="22" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="M22" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
@@ -4269,27 +4427,32 @@
       <c r="B23" s="52"/>
       <c r="C23" s="52"/>
       <c r="D23" s="22" t="s">
-        <v>164</v>
+        <v>151</v>
       </c>
       <c r="E23" s="22"/>
+      <c r="F23" s="22" t="s">
+        <v>76</v>
+      </c>
       <c r="G23" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="H23" s="22"/>
+      <c r="H23" s="22" t="s">
+        <v>36</v>
+      </c>
       <c r="I23" s="22" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="J23" s="22" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="K23" s="22" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="L23" s="22" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="M23" t="s">
-        <v>165</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -4299,28 +4462,32 @@
       <c r="B24" s="52"/>
       <c r="C24" s="52"/>
       <c r="D24" s="22" t="s">
-        <v>166</v>
+        <v>153</v>
       </c>
       <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
+      <c r="F24" s="22" t="s">
+        <v>76</v>
+      </c>
       <c r="G24" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="H24" s="22"/>
+      <c r="H24" s="22" t="s">
+        <v>36</v>
+      </c>
       <c r="I24" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="J24" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="K24" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="L24" s="22" t="s">
+        <v>497</v>
+      </c>
+      <c r="M24" t="s">
         <v>154</v>
-      </c>
-      <c r="J24" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="K24" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="L24" s="22" t="s">
-        <v>513</v>
-      </c>
-      <c r="M24" s="22" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -4330,28 +4497,30 @@
       <c r="B25" s="52"/>
       <c r="C25" s="52"/>
       <c r="D25" s="22" t="s">
-        <v>168</v>
+        <v>155</v>
       </c>
       <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
+      <c r="F25" s="22" t="s">
+        <v>76</v>
+      </c>
       <c r="G25" s="22" t="s">
         <v>35</v>
       </c>
       <c r="H25" s="22"/>
       <c r="I25" s="22" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="J25" s="22" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="K25" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="L25" s="22" t="s">
+        <v>497</v>
+      </c>
+      <c r="M25" t="s">
         <v>156</v>
-      </c>
-      <c r="L25" s="22" t="s">
-        <v>513</v>
-      </c>
-      <c r="M25" s="22" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -4361,28 +4530,30 @@
       <c r="B26" s="52"/>
       <c r="C26" s="52"/>
       <c r="D26" s="22" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
+      <c r="F26" s="22" t="s">
+        <v>76</v>
+      </c>
       <c r="G26" s="22" t="s">
         <v>35</v>
       </c>
       <c r="H26" s="22"/>
       <c r="I26" s="22" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="J26" s="22" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="K26" s="22" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="L26" s="22" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="M26" s="22" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -4390,36 +4561,32 @@
         <v>2</v>
       </c>
       <c r="B27" s="52"/>
-      <c r="C27" s="28" t="s">
-        <v>172</v>
-      </c>
+      <c r="C27" s="52"/>
       <c r="D27" s="22" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22" t="s">
-        <v>174</v>
+        <v>76</v>
       </c>
       <c r="G27" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="H27" s="22" t="s">
-        <v>36</v>
-      </c>
+      <c r="H27" s="22"/>
       <c r="I27" s="22" t="s">
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="J27" s="22" t="s">
-        <v>176</v>
+        <v>146</v>
       </c>
       <c r="K27" s="22" t="s">
-        <v>177</v>
+        <v>147</v>
       </c>
       <c r="L27" s="22" t="s">
-        <v>510</v>
+        <v>497</v>
       </c>
       <c r="M27" s="22" t="s">
-        <v>178</v>
+        <v>160</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -4427,11 +4594,9 @@
         <v>2</v>
       </c>
       <c r="B28" s="52"/>
-      <c r="C28" s="28" t="s">
-        <v>179</v>
-      </c>
+      <c r="C28" s="52"/>
       <c r="D28" s="22" t="s">
-        <v>180</v>
+        <v>161</v>
       </c>
       <c r="E28" s="22"/>
       <c r="F28" s="22" t="s">
@@ -4440,103 +4605,109 @@
       <c r="G28" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="H28" s="22" t="s">
-        <v>36</v>
-      </c>
+      <c r="H28" s="22"/>
       <c r="I28" s="22" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="J28" s="22" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="K28" s="22" t="s">
-        <v>181</v>
+        <v>147</v>
       </c>
       <c r="L28" s="22" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="M28" s="22" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="26">
-        <v>1</v>
-      </c>
-      <c r="B29" s="52" t="s">
-        <v>183</v>
-      </c>
-      <c r="C29" s="52" t="s">
-        <v>184</v>
+      <c r="A29" s="23">
+        <v>2</v>
+      </c>
+      <c r="B29" s="52"/>
+      <c r="C29" s="28" t="s">
+        <v>163</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="E29" s="22"/>
       <c r="F29" s="22" t="s">
-        <v>76</v>
+        <v>165</v>
       </c>
       <c r="G29" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="H29" s="22"/>
+        <v>35</v>
+      </c>
+      <c r="H29" s="22" t="s">
+        <v>36</v>
+      </c>
       <c r="I29" s="22" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="J29" s="22" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="K29" s="22" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="L29" s="22" t="s">
-        <v>513</v>
+        <v>496</v>
       </c>
       <c r="M29" s="22" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="26">
-        <v>1</v>
+      <c r="A30" s="23">
+        <v>2</v>
       </c>
       <c r="B30" s="52"/>
-      <c r="C30" s="52"/>
+      <c r="C30" s="28" t="s">
+        <v>170</v>
+      </c>
       <c r="D30" s="22" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="E30" s="22"/>
       <c r="F30" s="22" t="s">
         <v>76</v>
       </c>
       <c r="G30" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="H30" s="22"/>
+        <v>35</v>
+      </c>
+      <c r="H30" s="22" t="s">
+        <v>36</v>
+      </c>
       <c r="I30" s="22" t="s">
-        <v>186</v>
+        <v>145</v>
       </c>
       <c r="J30" s="22" t="s">
-        <v>187</v>
+        <v>146</v>
       </c>
       <c r="K30" s="22" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="L30" s="22" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="M30" s="22" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="26">
         <v>1</v>
       </c>
-      <c r="B31" s="52"/>
-      <c r="C31" s="52"/>
+      <c r="B31" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="C31" s="52" t="s">
+        <v>175</v>
+      </c>
       <c r="D31" s="22" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="E31" s="22"/>
       <c r="F31" s="22" t="s">
@@ -4547,191 +4718,191 @@
       </c>
       <c r="H31" s="22"/>
       <c r="I31" s="22" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="J31" s="22" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="K31" s="22" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="L31" s="22" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="M31" s="22" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="23">
-        <v>2</v>
+      <c r="A32" s="26">
+        <v>1</v>
       </c>
       <c r="B32" s="52"/>
-      <c r="C32" s="52" t="s">
-        <v>194</v>
-      </c>
+      <c r="C32" s="52"/>
       <c r="D32" s="22" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="E32" s="22"/>
       <c r="F32" s="22" t="s">
-        <v>174</v>
+        <v>76</v>
       </c>
       <c r="G32" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="H32" s="22" t="s">
-        <v>104</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="H32" s="22"/>
       <c r="I32" s="22" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="J32" s="22" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="K32" s="22" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="L32" s="22" t="s">
-        <v>514</v>
-      </c>
-      <c r="M32" s="22"/>
+        <v>497</v>
+      </c>
+      <c r="M32" s="22" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="23">
-        <v>2</v>
+      <c r="A33" s="26">
+        <v>1</v>
       </c>
       <c r="B33" s="52"/>
       <c r="C33" s="52"/>
       <c r="D33" s="22" t="s">
-        <v>200</v>
+        <v>183</v>
       </c>
       <c r="E33" s="22"/>
       <c r="F33" s="22" t="s">
-        <v>16</v>
+        <v>76</v>
       </c>
       <c r="G33" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="H33" s="22" t="s">
-        <v>36</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="H33" s="22"/>
       <c r="I33" s="22" t="s">
-        <v>202</v>
+        <v>177</v>
       </c>
       <c r="J33" s="22" t="s">
-        <v>203</v>
+        <v>178</v>
       </c>
       <c r="K33" s="22" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="L33" s="22" t="s">
-        <v>510</v>
+        <v>497</v>
       </c>
       <c r="M33" s="22" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="23">
         <v>2</v>
       </c>
-      <c r="B34" s="54" t="s">
-        <v>206</v>
-      </c>
-      <c r="C34" s="29" t="s">
-        <v>207</v>
+      <c r="B34" s="52"/>
+      <c r="C34" s="52" t="s">
+        <v>185</v>
       </c>
       <c r="D34" s="22" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="E34" s="22"/>
-      <c r="F34" t="s">
-        <v>209</v>
+      <c r="F34" s="22" t="s">
+        <v>165</v>
       </c>
       <c r="G34" s="22" t="s">
-        <v>210</v>
+        <v>187</v>
       </c>
       <c r="H34" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="I34" t="s">
-        <v>211</v>
-      </c>
-      <c r="J34" s="50" t="s">
-        <v>212</v>
-      </c>
-      <c r="K34" t="s">
-        <v>213</v>
+        <v>104</v>
+      </c>
+      <c r="I34" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="J34" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="K34" s="22" t="s">
+        <v>190</v>
       </c>
       <c r="L34" s="22" t="s">
-        <v>515</v>
-      </c>
+        <v>498</v>
+      </c>
+      <c r="M34" s="22"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="23">
         <v>2</v>
       </c>
-      <c r="B35" s="54"/>
-      <c r="C35" s="54" t="s">
-        <v>214</v>
-      </c>
+      <c r="B35" s="52"/>
+      <c r="C35" s="52"/>
       <c r="D35" s="22" t="s">
-        <v>215</v>
+        <v>191</v>
       </c>
       <c r="E35" s="22"/>
-      <c r="F35" t="s">
-        <v>209</v>
+      <c r="F35" s="22" t="s">
+        <v>16</v>
       </c>
       <c r="G35" s="22" t="s">
-        <v>210</v>
+        <v>192</v>
       </c>
       <c r="H35" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="I35" t="s">
-        <v>211</v>
-      </c>
-      <c r="J35" s="50" t="s">
-        <v>212</v>
-      </c>
-      <c r="K35" t="s">
-        <v>213</v>
+        <v>36</v>
+      </c>
+      <c r="I35" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="J35" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="K35" s="22" t="s">
+        <v>542</v>
       </c>
       <c r="L35" s="22" t="s">
-        <v>515</v>
+        <v>496</v>
+      </c>
+      <c r="M35" s="22" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="23">
         <v>2</v>
       </c>
-      <c r="B36" s="54"/>
-      <c r="C36" s="54"/>
+      <c r="B36" s="54" t="s">
+        <v>196</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>197</v>
+      </c>
       <c r="D36" s="22" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="E36" s="22"/>
       <c r="F36" t="s">
-        <v>209</v>
-      </c>
-      <c r="G36" t="s">
-        <v>210</v>
+        <v>199</v>
+      </c>
+      <c r="G36" s="22" t="s">
+        <v>200</v>
       </c>
       <c r="H36" s="22" t="s">
         <v>26</v>
       </c>
       <c r="I36" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="J36" s="50" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="K36" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L36" s="22" t="s">
-        <v>515</v>
+        <v>499</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
@@ -4739,31 +4910,33 @@
         <v>2</v>
       </c>
       <c r="B37" s="54"/>
-      <c r="C37" s="54"/>
+      <c r="C37" s="54" t="s">
+        <v>204</v>
+      </c>
       <c r="D37" s="22" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="E37" s="22"/>
       <c r="F37" t="s">
-        <v>209</v>
-      </c>
-      <c r="G37" t="s">
-        <v>210</v>
+        <v>199</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>200</v>
       </c>
       <c r="H37" s="22" t="s">
         <v>26</v>
       </c>
       <c r="I37" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="J37" s="50" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="K37" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L37" s="22" t="s">
-        <v>515</v>
+        <v>499</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
@@ -4771,33 +4944,31 @@
         <v>2</v>
       </c>
       <c r="B38" s="54"/>
-      <c r="C38" s="54" t="s">
-        <v>218</v>
-      </c>
+      <c r="C38" s="54"/>
       <c r="D38" s="22" t="s">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="E38" s="22"/>
       <c r="F38" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="G38" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="H38" s="22" t="s">
         <v>26</v>
       </c>
       <c r="I38" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="J38" s="50" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="K38" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L38" s="22" t="s">
-        <v>515</v>
+        <v>499</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
@@ -4807,55 +4978,121 @@
       <c r="B39" s="54"/>
       <c r="C39" s="54"/>
       <c r="D39" s="22" t="s">
-        <v>220</v>
+        <v>207</v>
       </c>
       <c r="E39" s="22"/>
       <c r="F39" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="G39" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="H39" s="22" t="s">
         <v>26</v>
       </c>
       <c r="I39" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="J39" s="50" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="K39" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="L39" s="22" t="s">
-        <v>515</v>
+        <v>499</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="23">
+        <v>2</v>
+      </c>
+      <c r="B40" s="54"/>
+      <c r="C40" s="54" t="s">
+        <v>208</v>
+      </c>
+      <c r="D40" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="E40" s="22"/>
+      <c r="F40" t="s">
+        <v>199</v>
+      </c>
+      <c r="G40" t="s">
+        <v>200</v>
+      </c>
+      <c r="H40" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I40" t="s">
+        <v>201</v>
+      </c>
+      <c r="J40" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="K40" t="s">
+        <v>203</v>
+      </c>
+      <c r="L40" s="22" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="23">
+        <v>2</v>
+      </c>
+      <c r="B41" s="54"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="E41" s="22"/>
+      <c r="F41" t="s">
+        <v>199</v>
+      </c>
+      <c r="G41" t="s">
+        <v>200</v>
+      </c>
+      <c r="H41" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="I41" t="s">
+        <v>201</v>
+      </c>
+      <c r="J41" s="50" t="s">
+        <v>202</v>
+      </c>
+      <c r="K41" t="s">
+        <v>203</v>
+      </c>
+      <c r="L41" s="22" t="s">
+        <v>499</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="B34:B39"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="B2:B12"/>
-    <mergeCell ref="B13:B18"/>
-    <mergeCell ref="B19:B28"/>
-    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="B14:B20"/>
+    <mergeCell ref="C15:C20"/>
+    <mergeCell ref="C21:C28"/>
+    <mergeCell ref="B21:B30"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="B36:B41"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="B2:B13"/>
+    <mergeCell ref="B31:B35"/>
     <mergeCell ref="C2:C5"/>
-    <mergeCell ref="C6:C8"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="C14:C18"/>
-    <mergeCell ref="C19:C26"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C31:C33"/>
+    <mergeCell ref="C37:C39"/>
+    <mergeCell ref="C6:C9"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J34" r:id="rId1" xr:uid="{3D79DC03-4AD8-4138-BA78-16543353E812}"/>
-    <hyperlink ref="J36" r:id="rId2" xr:uid="{2C5D8387-C3E7-4558-8512-24776549ECBC}"/>
-    <hyperlink ref="J38" r:id="rId3" xr:uid="{74409AF7-44EC-4DDA-94CE-5CFE6B6EF45D}"/>
-    <hyperlink ref="J39" r:id="rId4" xr:uid="{C809E76F-A449-46AC-8602-30F16878D60F}"/>
-    <hyperlink ref="J35" r:id="rId5" xr:uid="{E454A5A6-3A9A-4343-AB97-574D153141D3}"/>
-    <hyperlink ref="J37" r:id="rId6" xr:uid="{A9860B9E-3E33-44F9-9771-16C1931572D4}"/>
+    <hyperlink ref="J36" r:id="rId1" xr:uid="{3D79DC03-4AD8-4138-BA78-16543353E812}"/>
+    <hyperlink ref="J38" r:id="rId2" xr:uid="{2C5D8387-C3E7-4558-8512-24776549ECBC}"/>
+    <hyperlink ref="J40" r:id="rId3" xr:uid="{74409AF7-44EC-4DDA-94CE-5CFE6B6EF45D}"/>
+    <hyperlink ref="J41" r:id="rId4" xr:uid="{C809E76F-A449-46AC-8602-30F16878D60F}"/>
+    <hyperlink ref="J37" r:id="rId5" xr:uid="{E454A5A6-3A9A-4343-AB97-574D153141D3}"/>
+    <hyperlink ref="J39" r:id="rId6" xr:uid="{A9860B9E-3E33-44F9-9771-16C1931572D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4865,19 +5102,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9F95016-FFA1-D04E-AB0C-5DF6EE3EB4E3}">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomLeft" activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
     <col min="3" max="3" width="37.109375" customWidth="1"/>
-    <col min="4" max="4" width="39.109375" customWidth="1"/>
+    <col min="4" max="4" width="30.77734375" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="11" max="11" width="73.6640625" customWidth="1"/>
-    <col min="12" max="12" width="12.44140625" customWidth="1"/>
+    <col min="11" max="11" width="37.5546875" customWidth="1"/>
+    <col min="12" max="12" width="25.109375" customWidth="1"/>
     <col min="13" max="13" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4927,13 +5164,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="52" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="C2" s="52" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22" t="s">
@@ -4946,17 +5183,19 @@
         <v>36</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="J2" s="22" t="s">
         <v>43</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="L2" s="22"/>
+        <v>215</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>496</v>
+      </c>
       <c r="M2" s="22" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -4966,7 +5205,7 @@
       <c r="B3" s="52"/>
       <c r="C3" s="52"/>
       <c r="D3" s="22" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="22" t="s">
@@ -4979,17 +5218,19 @@
         <v>36</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="J3" s="22" t="s">
         <v>43</v>
       </c>
       <c r="K3" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="L3" s="22"/>
+        <v>215</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>496</v>
+      </c>
       <c r="M3" s="22" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -4997,36 +5238,38 @@
         <v>2</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="E4" s="22"/>
       <c r="F4" s="22" t="s">
         <v>76</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="H4" s="22" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="K4" s="22" t="s">
-        <v>236</v>
-      </c>
-      <c r="L4" s="22"/>
+        <v>226</v>
+      </c>
+      <c r="L4" s="22" t="s">
+        <v>506</v>
+      </c>
       <c r="M4" s="22" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -5035,7 +5278,7 @@
       </c>
       <c r="B5" s="52"/>
       <c r="C5" s="42" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="D5" s="43" t="s">
         <v>54</v>
@@ -5047,7 +5290,7 @@
       <c r="I5" s="34"/>
       <c r="J5" s="34"/>
       <c r="K5" s="34" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="L5" s="34"/>
       <c r="M5" s="25" t="s">
@@ -5060,10 +5303,10 @@
       </c>
       <c r="B6" s="52"/>
       <c r="C6" s="52" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="22" t="s">
@@ -5076,17 +5319,19 @@
         <v>36</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="K6" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="L6" s="22"/>
+        <v>215</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>507</v>
+      </c>
       <c r="M6" s="22" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -5096,7 +5341,7 @@
       <c r="B7" s="52"/>
       <c r="C7" s="52"/>
       <c r="D7" s="22" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="E7" s="22"/>
       <c r="F7" s="22" t="s">
@@ -5113,11 +5358,13 @@
         <v>38</v>
       </c>
       <c r="K7" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="L7" s="22"/>
+        <v>235</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>507</v>
+      </c>
       <c r="M7" s="22" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -5127,30 +5374,32 @@
       <c r="B8" s="52"/>
       <c r="C8" s="52"/>
       <c r="D8" s="22" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22" t="s">
         <v>76</v>
       </c>
       <c r="G8" s="22" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="H8" s="22" t="s">
         <v>36</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="K8" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="L8" s="22"/>
+        <v>215</v>
+      </c>
+      <c r="L8" s="22" t="s">
+        <v>506</v>
+      </c>
       <c r="M8" s="22" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -5160,30 +5409,32 @@
       <c r="B9" s="52"/>
       <c r="C9" s="52"/>
       <c r="D9" s="22" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="22" t="s">
         <v>76</v>
       </c>
       <c r="G9" s="22" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="H9" s="22" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="J9" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="K9" s="22" t="s">
         <v>235</v>
       </c>
-      <c r="K9" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="L9" s="22"/>
+      <c r="L9" s="22" t="s">
+        <v>506</v>
+      </c>
       <c r="M9" s="22" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
@@ -5193,30 +5444,32 @@
       <c r="B10" s="52"/>
       <c r="C10" s="52"/>
       <c r="D10" s="22" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="E10" s="22"/>
       <c r="F10" s="22" t="s">
         <v>76</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="H10" s="22" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="I10" s="22" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="J10" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="K10" s="22" t="s">
         <v>235</v>
       </c>
-      <c r="K10" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="L10" s="22"/>
+      <c r="L10" s="22" t="s">
+        <v>506</v>
+      </c>
       <c r="M10" s="22" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -5225,10 +5478,10 @@
       </c>
       <c r="B11" s="52"/>
       <c r="C11" s="39" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22" t="s">
@@ -5241,17 +5494,19 @@
         <v>36</v>
       </c>
       <c r="I11" s="22" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="J11" s="22" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>257</v>
-      </c>
-      <c r="L11" s="22"/>
+        <v>247</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>496</v>
+      </c>
       <c r="M11" s="22" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -5260,7 +5515,7 @@
       </c>
       <c r="B12" s="52"/>
       <c r="C12" s="42" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="D12" s="43" t="s">
         <v>54</v>
@@ -5272,7 +5527,7 @@
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
       <c r="K12" s="34" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="L12" s="34"/>
       <c r="M12" s="25" t="s">
@@ -5285,10 +5540,10 @@
       </c>
       <c r="B13" s="52"/>
       <c r="C13" s="51" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="E13" s="22"/>
       <c r="F13" s="22" t="s">
@@ -5298,20 +5553,22 @@
         <v>35</v>
       </c>
       <c r="H13" s="22" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>266</v>
-      </c>
-      <c r="L13" s="22"/>
+        <v>256</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>496</v>
+      </c>
       <c r="M13" s="22" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -5319,10 +5576,10 @@
         <v>54</v>
       </c>
       <c r="B14" s="54" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="D14" s="43" t="s">
         <v>54</v>
@@ -5345,7 +5602,7 @@
       </c>
       <c r="B15" s="54"/>
       <c r="C15" s="42" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="D15" s="43" t="s">
         <v>54</v>
@@ -5357,7 +5614,7 @@
       <c r="I15" s="34"/>
       <c r="J15" s="34"/>
       <c r="K15" s="34" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="L15" s="34"/>
       <c r="M15" s="25" t="s">
@@ -5370,7 +5627,7 @@
       </c>
       <c r="B16" s="54"/>
       <c r="C16" s="44" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="D16" s="43" t="s">
         <v>54</v>
@@ -5392,10 +5649,10 @@
         <v>54</v>
       </c>
       <c r="B17" s="28" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="C17" s="42" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="D17" s="43" t="s">
         <v>54</v>
@@ -5407,7 +5664,7 @@
       <c r="I17" s="34"/>
       <c r="J17" s="34"/>
       <c r="K17" s="34" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="L17" s="34"/>
       <c r="M17" s="25" t="s">
@@ -5419,10 +5676,10 @@
         <v>54</v>
       </c>
       <c r="B18" s="52" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="D18" s="43" t="s">
         <v>54</v>
@@ -5434,7 +5691,7 @@
       <c r="I18" s="20"/>
       <c r="J18" s="20"/>
       <c r="K18" s="20" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="L18" s="20"/>
       <c r="M18" s="25" t="s">
@@ -5447,7 +5704,7 @@
       </c>
       <c r="B19" s="52"/>
       <c r="C19" s="44" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="D19" s="43" t="s">
         <v>54</v>
@@ -5470,10 +5727,10 @@
       </c>
       <c r="B20" s="52"/>
       <c r="C20" s="54" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="E20" s="22"/>
       <c r="F20" s="22" t="s">
@@ -5490,11 +5747,13 @@
         <v>38</v>
       </c>
       <c r="K20" s="22" t="s">
-        <v>282</v>
-      </c>
-      <c r="L20" s="22"/>
+        <v>272</v>
+      </c>
+      <c r="L20" s="22" t="s">
+        <v>508</v>
+      </c>
       <c r="M20" s="22" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
@@ -5504,7 +5763,7 @@
       <c r="B21" s="52"/>
       <c r="C21" s="54"/>
       <c r="D21" s="22" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="E21" s="22"/>
       <c r="F21" s="22" t="s">
@@ -5521,11 +5780,13 @@
         <v>38</v>
       </c>
       <c r="K21" s="22" t="s">
-        <v>282</v>
-      </c>
-      <c r="L21" s="22"/>
+        <v>272</v>
+      </c>
+      <c r="L21" s="22" t="s">
+        <v>508</v>
+      </c>
       <c r="M21" s="22" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
@@ -5534,7 +5795,7 @@
       </c>
       <c r="B22" s="52"/>
       <c r="C22" s="44" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="D22" s="43" t="s">
         <v>54</v>
@@ -5546,7 +5807,7 @@
       <c r="I22" s="20"/>
       <c r="J22" s="20"/>
       <c r="K22" s="20" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="L22" s="20"/>
       <c r="M22" s="25" t="s">
@@ -5558,13 +5819,13 @@
         <v>3</v>
       </c>
       <c r="B23" s="52" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="C23" s="39" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="E23" s="22"/>
       <c r="F23" s="22" t="s">
@@ -5574,7 +5835,7 @@
         <v>35</v>
       </c>
       <c r="H23" s="22" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="I23" s="22" t="s">
         <v>37</v>
@@ -5582,8 +5843,11 @@
       <c r="J23" s="22" t="s">
         <v>38</v>
       </c>
+      <c r="L23" s="22" t="s">
+        <v>508</v>
+      </c>
       <c r="M23" s="22" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
@@ -5592,10 +5856,10 @@
       </c>
       <c r="B24" s="52"/>
       <c r="C24" s="52" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="E24" s="22"/>
       <c r="F24" s="22" t="s">
@@ -5605,19 +5869,22 @@
         <v>17</v>
       </c>
       <c r="H24" s="22" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="J24" s="22" t="s">
         <v>43</v>
       </c>
       <c r="K24" t="s">
-        <v>295</v>
+        <v>285</v>
+      </c>
+      <c r="L24" s="22" t="s">
+        <v>506</v>
       </c>
       <c r="M24" s="22" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
@@ -5627,7 +5894,7 @@
       <c r="B25" s="52"/>
       <c r="C25" s="52"/>
       <c r="D25" s="22" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="E25" s="22"/>
       <c r="F25" s="22" t="s">
@@ -5637,18 +5904,20 @@
         <v>17</v>
       </c>
       <c r="H25" s="22" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="J25" s="22" t="s">
         <v>43</v>
       </c>
       <c r="K25" s="22"/>
-      <c r="L25" s="22"/>
+      <c r="L25" s="22" t="s">
+        <v>496</v>
+      </c>
       <c r="M25" s="22" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.3">
@@ -5658,7 +5927,7 @@
       <c r="B26" s="52"/>
       <c r="C26" s="52"/>
       <c r="D26" s="22" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="E26" s="22"/>
       <c r="F26" s="22" t="s">
@@ -5669,17 +5938,19 @@
       </c>
       <c r="H26" s="22"/>
       <c r="I26" s="22" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="J26" s="22" t="s">
         <v>43</v>
       </c>
       <c r="K26" s="22" t="s">
-        <v>300</v>
-      </c>
-      <c r="L26" s="22"/>
+        <v>290</v>
+      </c>
+      <c r="L26" s="22" t="s">
+        <v>496</v>
+      </c>
       <c r="M26" s="22" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
@@ -5688,10 +5959,10 @@
       </c>
       <c r="B27" s="52"/>
       <c r="C27" s="40" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="E27" s="22"/>
       <c r="F27" s="22" t="s">
@@ -5708,11 +5979,13 @@
         <v>38</v>
       </c>
       <c r="K27" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="L27" s="22"/>
+        <v>235</v>
+      </c>
+      <c r="L27" s="22" t="s">
+        <v>508</v>
+      </c>
       <c r="M27" s="22" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -5721,7 +5994,7 @@
       </c>
       <c r="B28" s="52"/>
       <c r="C28" s="42" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="D28" s="43" t="s">
         <v>54</v>
@@ -5744,10 +6017,10 @@
       </c>
       <c r="B29" s="52"/>
       <c r="C29" s="52" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="E29" s="22"/>
       <c r="F29" s="22" t="s">
@@ -5757,7 +6030,7 @@
         <v>35</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="I29" s="22" t="s">
         <v>37</v>
@@ -5766,11 +6039,13 @@
         <v>38</v>
       </c>
       <c r="K29" s="22" t="s">
-        <v>308</v>
-      </c>
-      <c r="L29" s="22"/>
+        <v>298</v>
+      </c>
+      <c r="L29" s="22" t="s">
+        <v>496</v>
+      </c>
       <c r="M29" s="22" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.3">
@@ -5780,7 +6055,7 @@
       <c r="B30" s="52"/>
       <c r="C30" s="52"/>
       <c r="D30" s="22" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="E30" s="22"/>
       <c r="F30" s="22" t="s">
@@ -5790,7 +6065,7 @@
         <v>35</v>
       </c>
       <c r="H30" s="22" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="I30" s="22" t="s">
         <v>37</v>
@@ -5799,9 +6074,11 @@
         <v>38</v>
       </c>
       <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
+      <c r="L30" s="22" t="s">
+        <v>496</v>
+      </c>
       <c r="M30" s="22" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.3">
@@ -5811,7 +6088,7 @@
       <c r="B31" s="52"/>
       <c r="C31" s="52"/>
       <c r="D31" s="22" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="E31" s="22"/>
       <c r="F31" s="22" t="s">
@@ -5821,7 +6098,7 @@
         <v>35</v>
       </c>
       <c r="H31" s="22" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="I31" s="22" t="s">
         <v>37</v>
@@ -5830,9 +6107,11 @@
         <v>38</v>
       </c>
       <c r="K31" s="22"/>
-      <c r="L31" s="22"/>
+      <c r="L31" s="22" t="s">
+        <v>509</v>
+      </c>
       <c r="M31" s="22" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
@@ -5841,7 +6120,7 @@
       </c>
       <c r="B32" s="52"/>
       <c r="C32" s="38" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="D32" s="43" t="s">
         <v>54</v>
@@ -5853,9 +6132,11 @@
       <c r="I32" s="20"/>
       <c r="J32" s="20"/>
       <c r="K32" s="20" t="s">
-        <v>313</v>
-      </c>
-      <c r="L32" s="20"/>
+        <v>303</v>
+      </c>
+      <c r="L32" s="20" t="s">
+        <v>510</v>
+      </c>
       <c r="M32" s="25" t="s">
         <v>54</v>
       </c>
@@ -5865,10 +6146,10 @@
         <v>54</v>
       </c>
       <c r="B33" s="39" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="C33" s="42" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="D33" s="43" t="s">
         <v>54</v>
@@ -5914,8 +6195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345648BA-9C58-4148-8A4E-841344F5CF5C}">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5923,14 +6204,14 @@
     <col min="1" max="1" width="8.88671875" style="31"/>
     <col min="2" max="2" width="23.33203125" style="29" customWidth="1"/>
     <col min="3" max="3" width="37.88671875" style="29" customWidth="1"/>
-    <col min="4" max="4" width="52.44140625" customWidth="1"/>
+    <col min="4" max="4" width="46.88671875" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" customWidth="1"/>
     <col min="8" max="8" width="6.88671875" customWidth="1"/>
     <col min="9" max="9" width="7.5546875" customWidth="1"/>
     <col min="10" max="10" width="7.33203125" customWidth="1"/>
-    <col min="11" max="11" width="70.33203125" customWidth="1"/>
-    <col min="12" max="12" width="12.109375" customWidth="1"/>
+    <col min="11" max="11" width="54.109375" customWidth="1"/>
+    <col min="12" max="12" width="24.33203125" customWidth="1"/>
     <col min="13" max="13" width="29" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5980,13 +6261,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="C2" s="28" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22" t="s">
@@ -5999,17 +6280,19 @@
         <v>77</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>321</v>
-      </c>
-      <c r="L2" s="22"/>
+        <v>311</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>506</v>
+      </c>
       <c r="M2" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -6018,10 +6301,10 @@
       </c>
       <c r="B3" s="53"/>
       <c r="C3" s="28" t="s">
-        <v>323</v>
+        <v>313</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>324</v>
+        <v>314</v>
       </c>
       <c r="E3" s="22"/>
       <c r="F3" s="22" t="s">
@@ -6034,16 +6317,19 @@
         <v>77</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="K3" t="s">
-        <v>326</v>
+        <v>316</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>506</v>
       </c>
       <c r="M3" t="s">
-        <v>327</v>
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
@@ -6051,10 +6337,10 @@
         <v>54</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>328</v>
+        <v>318</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>329</v>
+        <v>319</v>
       </c>
       <c r="D4" s="34" t="s">
         <v>54</v>
@@ -6066,7 +6352,7 @@
       <c r="I4" s="34"/>
       <c r="J4" s="34"/>
       <c r="K4" s="34" t="s">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="L4" s="34"/>
     </row>
@@ -6076,7 +6362,7 @@
       </c>
       <c r="B5" s="55"/>
       <c r="C5" s="35" t="s">
-        <v>331</v>
+        <v>321</v>
       </c>
       <c r="D5" s="34" t="s">
         <v>54</v>
@@ -6096,7 +6382,7 @@
       </c>
       <c r="B6" s="55"/>
       <c r="C6" s="35" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="D6" s="34" t="s">
         <v>54</v>
@@ -6108,7 +6394,7 @@
       <c r="I6" s="34"/>
       <c r="J6" s="34"/>
       <c r="K6" s="34" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="L6" s="34"/>
     </row>
@@ -6118,7 +6404,7 @@
       </c>
       <c r="B7" s="55"/>
       <c r="C7" s="35" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="D7" s="34" t="s">
         <v>54</v>
@@ -6130,7 +6416,7 @@
       <c r="I7" s="34"/>
       <c r="J7" s="34"/>
       <c r="K7" s="34" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="L7" s="34"/>
     </row>
@@ -6139,17 +6425,17 @@
         <v>2</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>335</v>
+        <v>325</v>
       </c>
       <c r="C8" s="28" t="s">
-        <v>336</v>
+        <v>326</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>337</v>
+        <v>327</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="22" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G8" s="22" t="s">
         <v>35</v>
@@ -6158,17 +6444,17 @@
         <v>26</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>338</v>
+        <v>328</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>339</v>
-      </c>
-      <c r="K8" s="22" t="s">
-        <v>340</v>
-      </c>
-      <c r="L8" s="22"/>
+        <v>329</v>
+      </c>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22" t="s">
+        <v>496</v>
+      </c>
       <c r="M8" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
@@ -6176,10 +6462,10 @@
         <v>54</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="D9" s="34" t="s">
         <v>54</v>
@@ -6191,7 +6477,7 @@
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
       <c r="K9" s="34" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="L9" s="34"/>
     </row>
@@ -6200,13 +6486,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="E10" s="30"/>
       <c r="F10" s="30" t="s">
@@ -6225,9 +6511,11 @@
         <v>20</v>
       </c>
       <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
+      <c r="L10" s="30" t="s">
+        <v>511</v>
+      </c>
       <c r="M10" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
@@ -6235,13 +6523,13 @@
         <v>1</v>
       </c>
       <c r="B11" s="52" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
       <c r="E11" s="22"/>
       <c r="F11" s="22" t="s">
@@ -6260,10 +6548,13 @@
         <v>20</v>
       </c>
       <c r="K11" t="s">
-        <v>352</v>
+        <v>341</v>
+      </c>
+      <c r="L11" s="30" t="s">
+        <v>512</v>
       </c>
       <c r="M11" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
@@ -6272,10 +6563,10 @@
       </c>
       <c r="B12" s="52"/>
       <c r="C12" s="28" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="E12" s="22"/>
       <c r="F12" s="22" t="s">
@@ -6294,16 +6585,18 @@
         <v>20</v>
       </c>
       <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
+      <c r="L12" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M12" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="26"/>
       <c r="B13" s="52"/>
       <c r="C13" s="42" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="D13" s="34" t="s">
         <v>54</v>
@@ -6315,7 +6608,7 @@
       <c r="I13" s="34"/>
       <c r="J13" s="34"/>
       <c r="K13" s="34" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="L13" s="34"/>
       <c r="M13" s="34"/>
@@ -6326,10 +6619,10 @@
       </c>
       <c r="B14" s="52"/>
       <c r="C14" s="52" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="22" t="s">
@@ -6339,7 +6632,7 @@
         <v>17</v>
       </c>
       <c r="H14" s="22" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="I14" s="22" t="s">
         <v>67</v>
@@ -6348,9 +6641,11 @@
         <v>68</v>
       </c>
       <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
+      <c r="L14" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M14" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -6360,7 +6655,7 @@
       <c r="B15" s="52"/>
       <c r="C15" s="52"/>
       <c r="D15" s="22" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="22" t="s">
@@ -6370,7 +6665,7 @@
         <v>17</v>
       </c>
       <c r="H15" s="22" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="I15" s="22" t="s">
         <v>67</v>
@@ -6379,9 +6674,11 @@
         <v>68</v>
       </c>
       <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
+      <c r="L15" s="22" t="s">
+        <v>513</v>
+      </c>
       <c r="M15" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.3">
@@ -6390,7 +6687,7 @@
       </c>
       <c r="B16" s="52"/>
       <c r="C16" s="35" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
       <c r="D16" s="34" t="s">
         <v>54</v>
@@ -6402,19 +6699,21 @@
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
       <c r="K16" s="34" t="s">
-        <v>366</v>
-      </c>
-      <c r="L16" s="34"/>
+        <v>355</v>
+      </c>
+      <c r="L16" s="34" t="s">
+        <v>514</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="33" t="s">
         <v>54</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>367</v>
+        <v>356</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="D17" s="48" t="s">
         <v>54</v>
@@ -6426,7 +6725,7 @@
       <c r="I17" s="35"/>
       <c r="J17" s="35"/>
       <c r="K17" s="48" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c r="L17" s="35"/>
       <c r="M17" s="35"/>
@@ -6451,9 +6750,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FB29AFA-0DDE-5049-B8DC-113E6F66B101}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6463,8 +6762,8 @@
     <col min="3" max="3" width="29" style="29" customWidth="1"/>
     <col min="4" max="4" width="32.33203125" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="10" max="10" width="69.33203125" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" customWidth="1"/>
+    <col min="10" max="10" width="58.109375" customWidth="1"/>
+    <col min="11" max="11" width="23.5546875" customWidth="1"/>
     <col min="12" max="12" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6511,10 +6810,10 @@
         <v>54</v>
       </c>
       <c r="B2" s="54" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="C2" s="38" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="D2" t="s">
         <v>54</v>
@@ -6525,7 +6824,7 @@
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
       <c r="J2" s="20" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="K2" s="20"/>
       <c r="L2" s="20"/>
@@ -6536,7 +6835,7 @@
       </c>
       <c r="B3" s="54"/>
       <c r="C3" s="38" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="D3" t="s">
         <v>54</v>
@@ -6556,7 +6855,7 @@
       </c>
       <c r="B4" s="54"/>
       <c r="C4" s="38" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
       <c r="D4" t="s">
         <v>54</v>
@@ -6576,7 +6875,7 @@
       </c>
       <c r="B5" s="54"/>
       <c r="C5" s="38" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="D5" t="s">
         <v>54</v>
@@ -6596,10 +6895,10 @@
       </c>
       <c r="B6" s="54"/>
       <c r="C6" s="54" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="D6" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="E6" t="s">
         <v>16</v>
@@ -6608,7 +6907,7 @@
         <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="H6" t="s">
         <v>37</v>
@@ -6617,11 +6916,13 @@
         <v>38</v>
       </c>
       <c r="J6" t="s">
-        <v>378</v>
-      </c>
-      <c r="K6"/>
+        <v>367</v>
+      </c>
+      <c r="K6" t="s">
+        <v>515</v>
+      </c>
       <c r="L6" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6631,7 +6932,7 @@
       <c r="B7" s="54"/>
       <c r="C7" s="54"/>
       <c r="D7" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
@@ -6640,7 +6941,7 @@
         <v>35</v>
       </c>
       <c r="G7" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="H7" t="s">
         <v>37</v>
@@ -6649,11 +6950,13 @@
         <v>38</v>
       </c>
       <c r="J7" t="s">
-        <v>378</v>
-      </c>
-      <c r="K7"/>
+        <v>367</v>
+      </c>
+      <c r="K7" t="s">
+        <v>515</v>
+      </c>
       <c r="L7" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
     </row>
     <row r="8" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6662,7 +6965,7 @@
       </c>
       <c r="B8" s="54"/>
       <c r="C8" s="38" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="D8" t="s">
         <v>54</v>
@@ -6673,7 +6976,7 @@
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
       <c r="J8" s="20" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="K8" s="20"/>
       <c r="L8" s="20"/>
@@ -6684,7 +6987,7 @@
       </c>
       <c r="B9" s="54"/>
       <c r="C9" s="38" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
       <c r="D9" t="s">
         <v>54</v>
@@ -6695,7 +6998,7 @@
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
       <c r="J9" s="20" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="K9" s="20"/>
       <c r="L9" s="20"/>
@@ -6705,13 +7008,13 @@
         <v>2</v>
       </c>
       <c r="B10" s="54" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="D10" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="E10" t="s">
         <v>16</v>
@@ -6720,7 +7023,7 @@
         <v>35</v>
       </c>
       <c r="G10" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="H10" t="s">
         <v>19</v>
@@ -6729,11 +7032,13 @@
         <v>20</v>
       </c>
       <c r="J10" t="s">
-        <v>387</v>
-      </c>
-      <c r="K10"/>
+        <v>376</v>
+      </c>
+      <c r="K10" t="s">
+        <v>516</v>
+      </c>
       <c r="L10" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6742,10 +7047,10 @@
       </c>
       <c r="B11" s="54"/>
       <c r="C11" s="29" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="D11" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
       <c r="E11" t="s">
         <v>16</v>
@@ -6754,7 +7059,7 @@
         <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="H11" t="s">
         <v>19</v>
@@ -6763,9 +7068,11 @@
         <v>20</v>
       </c>
       <c r="J11"/>
-      <c r="K11"/>
+      <c r="K11" t="s">
+        <v>517</v>
+      </c>
       <c r="L11" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6774,10 +7081,10 @@
       </c>
       <c r="B12" s="54"/>
       <c r="C12" s="29" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
       <c r="D12" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="E12" t="s">
         <v>16</v>
@@ -6786,7 +7093,7 @@
         <v>17</v>
       </c>
       <c r="G12" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="H12" t="s">
         <v>19</v>
@@ -6795,9 +7102,11 @@
         <v>20</v>
       </c>
       <c r="J12"/>
-      <c r="K12"/>
+      <c r="K12" t="s">
+        <v>518</v>
+      </c>
       <c r="L12" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
     </row>
     <row r="13" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6806,7 +7115,7 @@
       </c>
       <c r="B13" s="54"/>
       <c r="C13" s="38" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="D13" t="s">
         <v>54</v>
@@ -6817,7 +7126,7 @@
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
       <c r="J13" s="20" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
       <c r="K13" s="20"/>
       <c r="L13" s="20"/>
@@ -6827,10 +7136,10 @@
         <v>54</v>
       </c>
       <c r="B14" s="54" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
       <c r="D14" s="41" t="s">
         <v>54</v>
@@ -6850,13 +7159,13 @@
       </c>
       <c r="B15" s="54"/>
       <c r="C15" s="54" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="D15" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
       <c r="E15" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="F15" t="s">
         <v>17</v>
@@ -6870,12 +7179,12 @@
       <c r="I15" t="s">
         <v>20</v>
       </c>
-      <c r="J15" t="s">
-        <v>401</v>
-      </c>
-      <c r="K15"/>
+      <c r="J15"/>
+      <c r="K15" t="s">
+        <v>496</v>
+      </c>
       <c r="L15" t="s">
-        <v>402</v>
+        <v>390</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6885,10 +7194,10 @@
       <c r="B16" s="54"/>
       <c r="C16" s="54"/>
       <c r="D16" t="s">
-        <v>403</v>
+        <v>391</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="F16" t="s">
         <v>17</v>
@@ -6902,12 +7211,12 @@
       <c r="I16" t="s">
         <v>20</v>
       </c>
-      <c r="J16" t="s">
-        <v>401</v>
-      </c>
-      <c r="K16"/>
+      <c r="J16"/>
+      <c r="K16" t="s">
+        <v>496</v>
+      </c>
       <c r="L16" t="s">
-        <v>404</v>
+        <v>392</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6917,10 +7226,10 @@
       <c r="B17" s="54"/>
       <c r="C17" s="54"/>
       <c r="D17" t="s">
-        <v>405</v>
+        <v>393</v>
       </c>
       <c r="E17" t="s">
-        <v>76</v>
+        <v>16</v>
       </c>
       <c r="F17" t="s">
         <v>17</v>
@@ -6934,12 +7243,12 @@
       <c r="I17" t="s">
         <v>20</v>
       </c>
-      <c r="J17" t="s">
-        <v>401</v>
-      </c>
-      <c r="K17"/>
+      <c r="J17"/>
+      <c r="K17" t="s">
+        <v>496</v>
+      </c>
       <c r="L17" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -6948,7 +7257,7 @@
       </c>
       <c r="B18" s="54"/>
       <c r="C18" s="38" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="D18" s="19" t="s">
         <v>54</v>
@@ -6967,13 +7276,13 @@
         <v>1</v>
       </c>
       <c r="B19" s="54" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="C19" s="54" t="s">
-        <v>409</v>
+        <v>397</v>
       </c>
       <c r="D19" t="s">
-        <v>410</v>
+        <v>398</v>
       </c>
       <c r="E19" t="s">
         <v>16</v>
@@ -6982,7 +7291,7 @@
         <v>35</v>
       </c>
       <c r="G19" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="H19" t="s">
         <v>37</v>
@@ -6991,9 +7300,11 @@
         <v>38</v>
       </c>
       <c r="J19"/>
-      <c r="K19"/>
+      <c r="K19" t="s">
+        <v>519</v>
+      </c>
       <c r="L19" t="s">
-        <v>411</v>
+        <v>399</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -7003,7 +7314,7 @@
       <c r="B20" s="54"/>
       <c r="C20" s="54"/>
       <c r="D20" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="E20" t="s">
         <v>16</v>
@@ -7012,7 +7323,7 @@
         <v>35</v>
       </c>
       <c r="G20" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="H20" t="s">
         <v>37</v>
@@ -7021,9 +7332,11 @@
         <v>38</v>
       </c>
       <c r="J20"/>
-      <c r="K20"/>
+      <c r="K20" t="s">
+        <v>519</v>
+      </c>
       <c r="L20" t="s">
-        <v>413</v>
+        <v>401</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -7032,7 +7345,7 @@
       </c>
       <c r="B21" s="54"/>
       <c r="C21" s="38" t="s">
-        <v>414</v>
+        <v>402</v>
       </c>
       <c r="D21" s="20" t="s">
         <v>54</v>
@@ -7043,7 +7356,7 @@
       <c r="H21" s="20"/>
       <c r="I21" s="20"/>
       <c r="J21" s="20" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="K21" s="20"/>
       <c r="L21" s="20"/>
@@ -7054,7 +7367,7 @@
       </c>
       <c r="B22" s="54"/>
       <c r="C22" s="38" t="s">
-        <v>416</v>
+        <v>404</v>
       </c>
       <c r="D22" s="20" t="s">
         <v>54</v>
@@ -7065,7 +7378,7 @@
       <c r="H22" s="20"/>
       <c r="I22" s="20"/>
       <c r="J22" s="20" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="K22" s="20"/>
       <c r="L22" s="20"/>
@@ -7076,7 +7389,7 @@
       </c>
       <c r="B23" s="54"/>
       <c r="C23" s="38" t="s">
-        <v>417</v>
+        <v>405</v>
       </c>
       <c r="D23" s="20" t="s">
         <v>54</v>
@@ -7087,7 +7400,7 @@
       <c r="H23" s="20"/>
       <c r="I23" s="20"/>
       <c r="J23" s="20" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="K23" s="20"/>
       <c r="L23" s="20"/>
@@ -7098,7 +7411,7 @@
       </c>
       <c r="B24" s="54"/>
       <c r="C24" s="38" t="s">
-        <v>418</v>
+        <v>406</v>
       </c>
       <c r="D24" s="20" t="s">
         <v>54</v>
@@ -7109,7 +7422,7 @@
       <c r="H24" s="20"/>
       <c r="I24" s="20"/>
       <c r="J24" s="20" t="s">
-        <v>415</v>
+        <v>403</v>
       </c>
       <c r="K24" s="20"/>
       <c r="L24" s="20"/>
@@ -7120,7 +7433,7 @@
       </c>
       <c r="B25" s="54"/>
       <c r="C25" s="38" t="s">
-        <v>419</v>
+        <v>407</v>
       </c>
       <c r="D25" s="20" t="s">
         <v>54</v>
@@ -7131,9 +7444,11 @@
       <c r="H25" s="20"/>
       <c r="I25" s="20"/>
       <c r="J25" s="20" t="s">
-        <v>420</v>
-      </c>
-      <c r="K25" s="20"/>
+        <v>408</v>
+      </c>
+      <c r="K25" s="20" t="s">
+        <v>520</v>
+      </c>
       <c r="L25" s="20"/>
     </row>
     <row r="26" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -7141,13 +7456,13 @@
         <v>1</v>
       </c>
       <c r="B26" s="54" t="s">
-        <v>421</v>
+        <v>409</v>
       </c>
       <c r="C26" s="54" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
       <c r="D26" t="s">
-        <v>423</v>
+        <v>411</v>
       </c>
       <c r="E26" t="s">
         <v>16</v>
@@ -7156,7 +7471,7 @@
         <v>35</v>
       </c>
       <c r="G26" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="H26" t="s">
         <v>37</v>
@@ -7165,11 +7480,13 @@
         <v>38</v>
       </c>
       <c r="J26" t="s">
-        <v>424</v>
-      </c>
-      <c r="K26"/>
+        <v>412</v>
+      </c>
+      <c r="K26" t="s">
+        <v>521</v>
+      </c>
       <c r="L26" t="s">
-        <v>425</v>
+        <v>413</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -7179,7 +7496,7 @@
       <c r="B27" s="54"/>
       <c r="C27" s="54"/>
       <c r="D27" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="E27" t="s">
         <v>16</v>
@@ -7188,7 +7505,7 @@
         <v>35</v>
       </c>
       <c r="G27" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="H27" t="s">
         <v>37</v>
@@ -7197,11 +7514,13 @@
         <v>38</v>
       </c>
       <c r="J27" t="s">
-        <v>424</v>
-      </c>
-      <c r="K27"/>
+        <v>412</v>
+      </c>
+      <c r="K27" t="s">
+        <v>521</v>
+      </c>
       <c r="L27" t="s">
-        <v>427</v>
+        <v>415</v>
       </c>
     </row>
     <row r="28" spans="1:12" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -7210,7 +7529,7 @@
       </c>
       <c r="B28" s="54"/>
       <c r="C28" s="38" t="s">
-        <v>428</v>
+        <v>416</v>
       </c>
       <c r="D28" t="s">
         <v>54</v>
@@ -7230,7 +7549,7 @@
       </c>
       <c r="B29" s="54"/>
       <c r="C29" s="38" t="s">
-        <v>429</v>
+        <v>417</v>
       </c>
       <c r="D29" t="s">
         <v>54</v>
@@ -7241,7 +7560,7 @@
       <c r="H29" s="20"/>
       <c r="I29" s="20"/>
       <c r="J29" s="20" t="s">
-        <v>430</v>
+        <v>418</v>
       </c>
       <c r="K29" s="20"/>
       <c r="L29" s="20"/>
@@ -7252,15 +7571,15 @@
       </c>
       <c r="B30" s="54"/>
       <c r="C30" s="29" t="s">
-        <v>431</v>
+        <v>419</v>
       </c>
       <c r="D30" t="s">
-        <v>432</v>
+        <v>420</v>
       </c>
       <c r="E30"/>
       <c r="F30"/>
       <c r="G30" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="H30" t="s">
         <v>42</v>
@@ -7269,11 +7588,13 @@
         <v>43</v>
       </c>
       <c r="J30" t="s">
-        <v>433</v>
-      </c>
-      <c r="K30"/>
+        <v>421</v>
+      </c>
+      <c r="K30" t="s">
+        <v>522</v>
+      </c>
       <c r="L30" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -7348,8 +7669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{514DD47A-AE44-4647-A357-A220BC698A77}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7360,18 +7681,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
-        <v>435</v>
+        <v>423</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="58" t="s">
-        <v>436</v>
+        <v>424</v>
       </c>
       <c r="B2" s="59"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="60" t="s">
-        <v>437</v>
+        <v>425</v>
       </c>
       <c r="B3" s="61"/>
     </row>
@@ -7381,13 +7702,13 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="60" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
       <c r="B5" s="61"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="56" t="s">
-        <v>439</v>
+        <v>427</v>
       </c>
       <c r="B6" s="57"/>
     </row>
@@ -7397,13 +7718,13 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="60" t="s">
-        <v>440</v>
+        <v>428</v>
       </c>
       <c r="B8" s="61"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="56" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="B9" s="57"/>
     </row>
@@ -7413,13 +7734,13 @@
     </row>
     <row r="11" spans="1:2" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="64" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="B11" s="65"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="66" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="B12" s="61"/>
     </row>
@@ -7429,36 +7750,36 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="60" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
       <c r="B14" s="61"/>
     </row>
     <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="62" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
       <c r="B15" s="63"/>
     </row>
     <row r="17" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>447</v>
+        <v>540</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -7466,7 +7787,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -7474,7 +7795,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -7482,7 +7803,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -7490,7 +7811,7 @@
         <v>6</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>453</v>
+        <v>440</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -7498,15 +7819,15 @@
         <v>7</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>454</v>
+        <v>441</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>455</v>
+        <v>442</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>456</v>
+        <v>443</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
@@ -7514,23 +7835,23 @@
         <v>0</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>457</v>
+        <v>444</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>459</v>
+        <v>446</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
-        <v>460</v>
+        <v>447</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>461</v>
+        <v>448</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -7539,16 +7860,16 @@
     </row>
     <row r="30" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>462</v>
+        <v>449</v>
       </c>
       <c r="B30" s="2"/>
     </row>
     <row r="31" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -7556,25 +7877,25 @@
         <v>54</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
-        <v>434</v>
+        <v>422</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>468</v>
+        <v>455</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -7647,13 +7968,13 @@
         <v>6</v>
       </c>
       <c r="F1" s="17" t="s">
-        <v>469</v>
+        <v>456</v>
       </c>
       <c r="G1" s="17" t="s">
         <v>10</v>
       </c>
       <c r="H1" s="17" t="s">
-        <v>458</v>
+        <v>445</v>
       </c>
       <c r="I1" s="17" t="s">
         <v>8</v>
@@ -7667,7 +7988,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>470</v>
+        <v>457</v>
       </c>
       <c r="D2" t="s">
         <v>16</v>
@@ -7679,32 +8000,32 @@
         <v>7</v>
       </c>
       <c r="H2" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>472</v>
+        <v>459</v>
       </c>
       <c r="C3" t="s">
-        <v>473</v>
+        <v>460</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="J3" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>476</v>
+        <v>463</v>
       </c>
       <c r="C4" t="s">
-        <v>477</v>
+        <v>464</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -7713,10 +8034,10 @@
         <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>478</v>
+        <v>465</v>
       </c>
       <c r="J4" t="s">
-        <v>479</v>
+        <v>466</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
@@ -7724,7 +8045,7 @@
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>480</v>
+        <v>467</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
@@ -7735,27 +8056,27 @@
     </row>
     <row r="6" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>481</v>
+        <v>468</v>
       </c>
       <c r="C6" t="s">
-        <v>482</v>
+        <v>469</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
       </c>
       <c r="I6" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="J6" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>483</v>
+        <v>470</v>
       </c>
       <c r="C7" t="s">
-        <v>484</v>
+        <v>471</v>
       </c>
       <c r="D7" t="s">
         <v>16</v>
@@ -7764,7 +8085,7 @@
         <v>17</v>
       </c>
       <c r="G7" t="s">
-        <v>485</v>
+        <v>472</v>
       </c>
       <c r="I7" t="s">
         <v>19</v>
@@ -7775,71 +8096,71 @@
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>486</v>
+        <v>473</v>
       </c>
       <c r="C8" t="s">
-        <v>487</v>
+        <v>474</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
       </c>
       <c r="I8" t="s">
-        <v>474</v>
+        <v>461</v>
       </c>
       <c r="J8" t="s">
-        <v>475</v>
+        <v>462</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>488</v>
+        <v>475</v>
       </c>
       <c r="B9" t="s">
-        <v>489</v>
+        <v>476</v>
       </c>
       <c r="H9" t="s">
-        <v>490</v>
+        <v>477</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>488</v>
+        <v>475</v>
       </c>
       <c r="B10" t="s">
-        <v>491</v>
+        <v>478</v>
       </c>
       <c r="H10" t="s">
-        <v>492</v>
+        <v>479</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>488</v>
+        <v>475</v>
       </c>
       <c r="B11" t="s">
-        <v>493</v>
+        <v>480</v>
       </c>
       <c r="G11" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>495</v>
+        <v>482</v>
       </c>
       <c r="G12" t="s">
-        <v>494</v>
+        <v>481</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>488</v>
+        <v>475</v>
       </c>
       <c r="B13" t="s">
-        <v>496</v>
+        <v>483</v>
       </c>
       <c r="G13" t="s">
-        <v>497</v>
+        <v>484</v>
       </c>
     </row>
   </sheetData>

</xml_diff>